<commit_message>
This log entry is for the previous commit as well as this one. CW3MdigitalHandbook.docx - Update thermal energy budget for NSantiam. FLOWreports_NSantiam.xml - Reorder the columns in the yearly thermal energy budget report. Flow.c, .h - Replace ReachSubnode::m_addedVolumeWP with m_addedVolYTD_WP. Add ReachSubnode::m_addedVolTodayWP. In FlowModel::StartStep(), add logic to zero out pNode->m_addedVolTodayWP. In FlowModel::MagicReachWaterReport_m3(), instead of putting added volume year-to-date into ReachADDED_VOL, put in reachAddedVolumeToday_m3. FluxExpr.cpp - Comment out the special logic for Clear Lake in Spring::Step(). ReachRouting.cpp - In ReachRouting::Step(), save node_current_added_volume to pNode->m_addedVolTodayWP. HBV.csv - Replace "NAME34" with "Walterville34".
</commit_message>
<xml_diff>
--- a/DataCW3M/SkillAssessment/Flow24monthsStatisticsCalculator.xlsx
+++ b/DataCW3M/SkillAssessment/Flow24monthsStatisticsCalculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\SkillAssessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F868D24-510F-4BB7-9538-9D36432B0C91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035B4E70-32A5-4EA7-8F0B-3D5DAA4BAB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics calculator" sheetId="1" r:id="rId1"/>
@@ -220,10 +220,10 @@
     <t>Phi =</t>
   </si>
   <si>
-    <t xml:space="preserve"> USGS_14158790_flow_SMITH RIVER ABV SMITH R RESV NR BELKNAP SPRINGS_23773393</t>
+    <t xml:space="preserve"> USGS_14178000_flow_NO SANTIAM R BLW BOULDER CRK  NR DETROIT  OR_23780591</t>
   </si>
   <si>
-    <t xml:space="preserve"> Obs:..\Observations\McKenzie\USGS_14158790_flow_SMITH RIVER ABV SMITH R RESV NR BELKNAP SPRINGS_23773393.csv</t>
+    <t xml:space="preserve"> Obs:..\Observations\NSantiam\USGS_14178000_flow_NO SANTIAM R BLW BOULDER CRK  NR DETROIT  OR_23780591.csv</t>
   </si>
 </sst>
 </file>
@@ -873,7 +873,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> USGS_14158790_flow_SMITH RIVER ABV SMITH R RESV NR BELKNAP SPRINGS_23773393</c:v>
+                  <c:v> USGS_14178000_flow_NO SANTIAM R BLW BOULDER CRK  NR DETROIT  OR_23780591</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -897,76 +897,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>546.36248799999998</c:v>
+                  <c:v>1318.969116</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>151.31860399999999</c:v>
+                  <c:v>654.81872599999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>126.125244</c:v>
+                  <c:v>1309.1667480000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>302.29577599999999</c:v>
+                  <c:v>2291.9421390000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>65.588188000000002</c:v>
+                  <c:v>1116.070923</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.867927999999999</c:v>
+                  <c:v>641.40801999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.077047</c:v>
+                  <c:v>464.63085899999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28.634432</c:v>
+                  <c:v>389.180969</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37.912457000000003</c:v>
+                  <c:v>435.92251599999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>47.509017999999998</c:v>
+                  <c:v>543.51409899999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33.267887000000002</c:v>
+                  <c:v>373.34747299999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>46.792563999999999</c:v>
+                  <c:v>508.02227800000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>130.10072299999999</c:v>
+                  <c:v>1263.4288329999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>149.669693</c:v>
+                  <c:v>1465.9085689999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>111.083878</c:v>
+                  <c:v>912.38482699999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>111.655807</c:v>
+                  <c:v>1197.2650149999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>83.535933999999997</c:v>
+                  <c:v>999.23718299999996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>80.034828000000005</c:v>
+                  <c:v>679.75945999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>37.069251999999999</c:v>
+                  <c:v>423.25503500000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>29.737268</c:v>
+                  <c:v>356.11215199999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29.753796000000001</c:v>
+                  <c:v>336.58340500000003</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>40.054530999999997</c:v>
+                  <c:v>439.83184799999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>76.444336000000007</c:v>
+                  <c:v>772.81073000000004</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>162.62640400000001</c:v>
+                  <c:v>1337.5745850000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -987,7 +987,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> Obs:..\Observations\McKenzie\USGS_14158790_flow_SMITH RIVER ABV SMITH R RESV NR BELKNAP SPRINGS_23773393.csv</c:v>
+                  <c:v> Obs:..\Observations\NSantiam\USGS_14178000_flow_NO SANTIAM R BLW BOULDER CRK  NR DETROIT  OR_23780591.csv</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1011,76 +1011,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>110.897835</c:v>
+                  <c:v>1057.9149170000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.155521</c:v>
+                  <c:v>726.88659700000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48.151909000000003</c:v>
+                  <c:v>751.378784</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>319.90457199999997</c:v>
+                  <c:v>2731.420654</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70.348693999999995</c:v>
+                  <c:v>1012.70343</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.041027</c:v>
+                  <c:v>639.75982699999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.6241539999999999</c:v>
+                  <c:v>461.15029900000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.368989</c:v>
+                  <c:v>373.73623700000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.4869310000000002</c:v>
+                  <c:v>386.91287199999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17.277432999999998</c:v>
+                  <c:v>432.39080799999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.1697410000000001</c:v>
+                  <c:v>381.75524899999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>48.831223000000001</c:v>
+                  <c:v>536.34008800000004</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>137.00288399999999</c:v>
+                  <c:v>1170.87085</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>131.610962</c:v>
+                  <c:v>1254.3043210000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>60.719954999999999</c:v>
+                  <c:v>690.69152799999995</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>148.37773100000001</c:v>
+                  <c:v>1226.988159</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>104.30669399999999</c:v>
+                  <c:v>1157.6922609999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>57.712505</c:v>
+                  <c:v>827.918274</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13.518675</c:v>
+                  <c:v>526.04125999999997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.8387399999999996</c:v>
+                  <c:v>416.39163200000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.014062</c:v>
+                  <c:v>381.95684799999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.5922260000000001</c:v>
+                  <c:v>418.79754600000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>61.275429000000003</c:v>
+                  <c:v>742.23394800000005</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>148.006989</c:v>
+                  <c:v>1301.7392580000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7261,7 +7261,7 @@
   <dimension ref="A1:AD3182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I27"/>
+      <selection activeCell="H3" sqref="H3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7280,7 +7280,7 @@
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="H1">
         <f>AVERAGE(H4:H15)</f>
-        <v>121.14596941666666</v>
+        <v>837.24948883333343</v>
       </c>
       <c r="I1"/>
       <c r="J1"/>
@@ -7289,7 +7289,7 @@
       </c>
       <c r="P1" s="11">
         <f>SUM(P4:P27)</f>
-        <v>219692.40428343348</v>
+        <v>773525.67325483949</v>
       </c>
       <c r="S1" t="s">
         <v>33</v>
@@ -7308,7 +7308,7 @@
       </c>
       <c r="B2" s="14">
         <f>H2-I2</f>
-        <v>37.970133416666656</v>
+        <v>25.965410874999861</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -7318,11 +7318,11 @@
       <c r="G2"/>
       <c r="H2">
         <f>AVERAGE(H4:H27)</f>
-        <v>103.97992012499999</v>
+        <v>842.96439616666669</v>
       </c>
       <c r="I2">
         <f>AVERAGE(I4:I27)</f>
-        <v>66.009786708333337</v>
+        <v>816.99898529166683</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -7332,12 +7332,12 @@
       <c r="O2" s="4"/>
       <c r="P2" s="4">
         <f>AVERAGE(P4:P27)</f>
-        <v>9153.8501784763957</v>
+        <v>32230.236385618311</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4">
         <f>AVERAGE(R4:R27)</f>
-        <v>45.370367249999994</v>
+        <v>117.05275720833329</v>
       </c>
       <c r="S2">
         <f>AVERAGE(S4:S27)</f>
@@ -7356,11 +7356,11 @@
       </c>
       <c r="B3" s="9">
         <f>(I2-H2)/H2</f>
-        <v>-0.3651679417624159</v>
+        <v>-3.0802500073640254E-2</v>
       </c>
       <c r="C3" s="16" t="str">
         <f>IF(ABS(B3)&lt;5%,"VG",IF(ABS(B3)&lt;10%,"G",IF(ABS(B3)&lt;15%,"S","NS")))</f>
-        <v>NS</v>
+        <v>VG</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>0</v>
@@ -7442,13 +7442,13 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="10">
         <f>1-SUM(P4:P27)/SUM(M4:M27)</f>
-        <v>-0.76324658183771477</v>
+        <v>0.87482661896324188</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>IF(B4&gt;0.8,"VG",IF(B4&gt;0.7,"G",IF(B4&gt;0.45,"S","NS")))</f>
-        <v>NS</v>
+        <v>VG</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -7463,46 +7463,46 @@
         <v>31</v>
       </c>
       <c r="H4">
-        <v>546.36248799999998</v>
+        <v>1318.969116</v>
       </c>
       <c r="I4">
-        <v>110.897835</v>
+        <v>1057.9149170000001</v>
       </c>
       <c r="J4" s="2">
         <f>I4-H4</f>
-        <v>-435.464653</v>
+        <v>-261.05419899999993</v>
       </c>
       <c r="K4" s="2">
         <f>I4-I$2</f>
-        <v>44.888048291666664</v>
+        <v>240.91593170833323</v>
       </c>
       <c r="L4" s="2">
         <f>H4-H$2</f>
-        <v>442.38256787500001</v>
+        <v>476.0047198333333</v>
       </c>
       <c r="M4" s="2">
         <f>K4*K4</f>
-        <v>2014.9368794349984</v>
+        <v>58040.486150894285</v>
       </c>
       <c r="N4" s="2">
         <f>L4*L4</f>
-        <v>195702.336359679</v>
+        <v>226580.49330361013</v>
       </c>
       <c r="O4" s="2">
         <f>K4*L4</f>
-        <v>19857.690070164506</v>
+        <v>114677.12057621162</v>
       </c>
       <c r="P4" s="2">
         <f>J4*J4</f>
-        <v>189629.4640124104</v>
+        <v>68149.294815531568</v>
       </c>
       <c r="Q4" s="2">
         <f>(I4-H$2)*(I4-H$2)</f>
-        <v>47.857546217746375</v>
+        <v>46203.72640652128</v>
       </c>
       <c r="R4" s="2">
         <f>ABS(J4)</f>
-        <v>435.464653</v>
+        <v>261.05419899999993</v>
       </c>
       <c r="S4">
         <v>5.1376660000000003</v>
@@ -7543,11 +7543,11 @@
       </c>
       <c r="B5" s="13">
         <f>SQRT(SUM(P4:P27))/SQRT(SUM(Q4:Q27))</f>
-        <v>1.1747356900297576</v>
+        <v>0.35333621499876455</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>IF(B5&lt;=0.5,"VG",IF(B5&lt;=0.6,"G",IF(B5&lt;=0.7,"S","NS")))</f>
-        <v>NS</v>
+        <v>VG</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -7562,46 +7562,46 @@
         <v>28</v>
       </c>
       <c r="H5">
-        <v>151.31860399999999</v>
+        <v>654.81872599999997</v>
       </c>
       <c r="I5">
-        <v>46.155521</v>
+        <v>726.88659700000005</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" ref="J5:J15" si="0">I5-H5</f>
-        <v>-105.163083</v>
+        <v>72.067871000000082</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" ref="K5:K15" si="1">I5-I$2</f>
-        <v>-19.854265708333337</v>
+        <v>-90.112388291666775</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" ref="L5:L15" si="2">H5-H$2</f>
-        <v>47.338683875000001</v>
+        <v>-188.14567016666672</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" ref="M5:M15" si="3">K5*K5</f>
-        <v>394.19186681710107</v>
+        <v>8120.2425236281233</v>
       </c>
       <c r="N5" s="2">
         <f t="shared" ref="N5:N15" si="4">L5*L5</f>
-        <v>2240.9509910171851</v>
+        <v>35398.793202464141</v>
       </c>
       <c r="O5" s="2">
         <f t="shared" ref="O5:O15" si="5">K5*L5</f>
-        <v>-939.87480793704481</v>
+        <v>16954.255685454536</v>
       </c>
       <c r="P5" s="2">
         <f t="shared" ref="P5:P15" si="6">J5*J5</f>
-        <v>11059.27402606489</v>
+        <v>5193.778030472653</v>
       </c>
       <c r="Q5" s="2">
         <f t="shared" ref="Q5:Q15" si="7">(I5-H$2)*(I5-H$2)</f>
-        <v>3343.6611341672997</v>
+        <v>13474.055459376994</v>
       </c>
       <c r="R5" s="2">
         <f t="shared" ref="R5:R15" si="8">ABS(J5)</f>
-        <v>105.163083</v>
+        <v>72.067871000000082</v>
       </c>
       <c r="S5">
         <v>5.2818040000000002</v>
@@ -7642,11 +7642,11 @@
       </c>
       <c r="B6" s="10">
         <f>B12*B12</f>
-        <v>0.38023983543207673</v>
+        <v>0.87745510124463066</v>
       </c>
       <c r="C6" s="7" t="str">
         <f>IF(B6&gt;0.85,"VG",IF(B6&gt;0.75,"G",IF(B6&gt;0.6,"S","NS")))</f>
-        <v>NS</v>
+        <v>VG</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -7661,46 +7661,46 @@
         <v>31</v>
       </c>
       <c r="H6">
-        <v>126.125244</v>
+        <v>1309.1667480000001</v>
       </c>
       <c r="I6">
-        <v>48.151909000000003</v>
+        <v>751.378784</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="0"/>
-        <v>-77.973334999999992</v>
+        <v>-557.7879640000001</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" si="1"/>
-        <v>-17.857877708333334</v>
+        <v>-65.620201291666831</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" si="2"/>
-        <v>22.145323875000003</v>
+        <v>466.20235183333341</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" si="3"/>
-        <v>318.90379624578861</v>
+        <v>4306.010817558873</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" si="4"/>
-        <v>490.4153695286451</v>
+        <v>217344.6328549312</v>
       </c>
       <c r="O6" s="2">
         <f t="shared" si="5"/>
-        <v>-395.46848557118449</v>
+        <v>-30592.292169951819</v>
       </c>
       <c r="P6" s="2">
         <f t="shared" si="6"/>
-        <v>6079.840971022224</v>
+        <v>311127.4127832654</v>
       </c>
       <c r="Q6" s="2">
         <f t="shared" si="7"/>
-        <v>3116.7668261731224</v>
+        <v>8387.9243559430852</v>
       </c>
       <c r="R6" s="2">
         <f t="shared" si="8"/>
-        <v>77.973334999999992</v>
+        <v>557.7879640000001</v>
       </c>
       <c r="S6">
         <v>5.855613</v>
@@ -7741,7 +7741,7 @@
       </c>
       <c r="B7" s="1">
         <f>H2</f>
-        <v>103.97992012499999</v>
+        <v>842.96439616666669</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7">
@@ -7757,46 +7757,46 @@
         <v>30</v>
       </c>
       <c r="H7">
-        <v>302.29577599999999</v>
+        <v>2291.9421390000002</v>
       </c>
       <c r="I7">
-        <v>319.90457199999997</v>
+        <v>2731.420654</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>17.608795999999984</v>
+        <v>439.47851499999979</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" si="1"/>
-        <v>253.89478529166664</v>
+        <v>1914.4216687083331</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" si="2"/>
-        <v>198.31585587500001</v>
+        <v>1448.9777428333337</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" si="3"/>
-        <v>64462.561998301499</v>
+        <v>3665010.3256199984</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" si="4"/>
-        <v>39329.178691433779</v>
+        <v>2099536.4992263825</v>
       </c>
       <c r="O7" s="2">
         <f t="shared" si="5"/>
-        <v>50351.361647316233</v>
+        <v>2773954.3883562246</v>
       </c>
       <c r="P7" s="2">
         <f t="shared" si="6"/>
-        <v>310.06969656961542</v>
+        <v>193141.36514660504</v>
       </c>
       <c r="Q7" s="2">
         <f t="shared" si="7"/>
-        <v>46623.455287339937</v>
+        <v>3566267.0377498777</v>
       </c>
       <c r="R7" s="2">
         <f t="shared" si="8"/>
-        <v>17.608795999999984</v>
+        <v>439.47851499999979</v>
       </c>
       <c r="S7">
         <v>6.2127059999999998</v>
@@ -7837,7 +7837,7 @@
       </c>
       <c r="B8" s="1">
         <f>_xlfn.STDEV.P(H4:H27)</f>
-        <v>111.47193190106964</v>
+        <v>476.93214122539456</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8">
@@ -7853,46 +7853,46 @@
         <v>31</v>
       </c>
       <c r="H8">
-        <v>65.588188000000002</v>
+        <v>1116.070923</v>
       </c>
       <c r="I8">
-        <v>70.348693999999995</v>
+        <v>1012.70343</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>4.7605059999999924</v>
+        <v>-103.36749299999997</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="1"/>
-        <v>4.3389072916666578</v>
+        <v>195.7044447083332</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" si="2"/>
-        <v>-38.39173212499999</v>
+        <v>273.10652683333331</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="3"/>
-        <v>18.826116485678092</v>
+        <v>38300.229678597047</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" si="4"/>
-        <v>1473.9250955577563</v>
+        <v>74587.174998966206</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" si="5"/>
-        <v>-166.57816645687552</v>
+        <v>53448.161180138995</v>
       </c>
       <c r="P8" s="2">
         <f t="shared" si="6"/>
-        <v>22.662417376035926</v>
+        <v>10684.838609105042</v>
       </c>
       <c r="Q8" s="2">
         <f t="shared" si="7"/>
-        <v>1131.0593706708823</v>
+        <v>28811.339606673479</v>
       </c>
       <c r="R8" s="2">
         <f t="shared" si="8"/>
-        <v>4.7605059999999924</v>
+        <v>103.36749299999997</v>
       </c>
       <c r="S8">
         <v>6.9663380000000004</v>
@@ -7933,7 +7933,7 @@
       </c>
       <c r="B9" s="1">
         <f>I2</f>
-        <v>66.009786708333337</v>
+        <v>816.99898529166683</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9">
@@ -7949,46 +7949,46 @@
         <v>30</v>
       </c>
       <c r="H9">
-        <v>37.867927999999999</v>
+        <v>641.40801999999996</v>
       </c>
       <c r="I9">
-        <v>18.041027</v>
+        <v>639.75982699999997</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>-19.826900999999999</v>
+        <v>-1.648192999999992</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="1"/>
-        <v>-47.968759708333337</v>
+        <v>-177.23915829166685</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" si="2"/>
-        <v>-66.111992125</v>
+        <v>-201.55637616666672</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" si="3"/>
-        <v>2301.0019079558238</v>
+        <v>31413.719231938539</v>
       </c>
       <c r="N9" s="2">
         <f t="shared" si="4"/>
-        <v>4370.7955027360622</v>
+        <v>40624.972773438858</v>
       </c>
       <c r="O9" s="2">
         <f t="shared" si="5"/>
-        <v>3171.3102640833508</v>
+        <v>35723.682460098593</v>
       </c>
       <c r="P9" s="2">
         <f t="shared" si="6"/>
-        <v>393.10600326380097</v>
+        <v>2.7165401652489738</v>
       </c>
       <c r="Q9" s="2">
         <f t="shared" si="7"/>
-        <v>7385.4933515501707</v>
+        <v>41292.096930210639</v>
       </c>
       <c r="R9" s="2">
         <f t="shared" si="8"/>
-        <v>19.826900999999999</v>
+        <v>1.648192999999992</v>
       </c>
       <c r="S9">
         <v>8.0567130000000002</v>
@@ -8029,7 +8029,7 @@
       </c>
       <c r="B10" s="1">
         <f>_xlfn.STDEV.P(I4:I27)</f>
-        <v>72.051889567013248</v>
+        <v>507.42954910553692</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -8044,46 +8044,46 @@
         <v>31</v>
       </c>
       <c r="H10">
-        <v>30.077047</v>
+        <v>464.63085899999999</v>
       </c>
       <c r="I10">
-        <v>6.6241539999999999</v>
+        <v>461.15029900000002</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="0"/>
-        <v>-23.452893</v>
+        <v>-3.4805599999999686</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="1"/>
-        <v>-59.38563270833334</v>
+        <v>-355.84868629166681</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" si="2"/>
-        <v>-73.902873124999985</v>
+        <v>-378.3335371666667</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" si="3"/>
-        <v>3526.6533721690707</v>
+        <v>126628.28753550509</v>
       </c>
       <c r="N10" s="2">
         <f t="shared" si="4"/>
-        <v>5461.6346561298451</v>
+        <v>143136.26534504158</v>
       </c>
       <c r="O10" s="2">
         <f t="shared" si="5"/>
-        <v>4388.7688794918076</v>
+        <v>134629.49218083784</v>
       </c>
       <c r="P10" s="2">
         <f t="shared" si="6"/>
-        <v>550.038190069449</v>
+        <v>12.114297913599781</v>
       </c>
       <c r="Q10" s="2">
         <f t="shared" si="7"/>
-        <v>9478.1451977856959</v>
+        <v>145782.00479519679</v>
       </c>
       <c r="R10" s="2">
         <f t="shared" si="8"/>
-        <v>23.452893</v>
+        <v>3.4805599999999686</v>
       </c>
       <c r="S10">
         <v>10.862743</v>
@@ -8124,7 +8124,7 @@
       </c>
       <c r="B11" s="1">
         <f>SQRT(P$2)</f>
-        <v>95.675755437186879</v>
+        <v>179.52781507504153</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -8139,46 +8139,46 @@
         <v>31</v>
       </c>
       <c r="H11">
-        <v>28.634432</v>
+        <v>389.180969</v>
       </c>
       <c r="I11">
-        <v>3.368989</v>
+        <v>373.73623700000002</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
-        <v>-25.265443000000001</v>
+        <v>-15.444731999999988</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" si="1"/>
-        <v>-62.640797708333338</v>
+        <v>-443.26274829166681</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" si="2"/>
-        <v>-75.345488124999989</v>
+        <v>-453.78342716666668</v>
       </c>
       <c r="M11" s="2">
         <f t="shared" si="3"/>
-        <v>3923.8695375363391</v>
+        <v>196481.86402308158</v>
       </c>
       <c r="N11" s="2">
         <f t="shared" si="4"/>
-        <v>5676.9425807945145</v>
+        <v>205919.39877112547</v>
       </c>
       <c r="O11" s="2">
         <f t="shared" si="5"/>
-        <v>4719.7014798737564</v>
+        <v>201145.28905510809</v>
       </c>
       <c r="P11" s="2">
         <f t="shared" si="6"/>
-        <v>638.34260998624904</v>
+        <v>238.53974655182361</v>
       </c>
       <c r="Q11" s="2">
         <f t="shared" si="7"/>
-        <v>10122.559461839492</v>
+        <v>220175.06535493868</v>
       </c>
       <c r="R11" s="2">
         <f t="shared" si="8"/>
-        <v>25.265443000000001</v>
+        <v>15.444731999999988</v>
       </c>
       <c r="S11">
         <v>13.279059</v>
@@ -8219,7 +8219,7 @@
       </c>
       <c r="B12" s="1">
         <f>SUM(O4:O27)/SQRT(SUM(M4:M27)*SUM(N4:N27))</f>
-        <v>0.6166359018351727</v>
+        <v>0.93672573427051242</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12">
@@ -8235,46 +8235,46 @@
         <v>30</v>
       </c>
       <c r="H12">
-        <v>37.912457000000003</v>
+        <v>435.92251599999997</v>
       </c>
       <c r="I12">
-        <v>6.4869310000000002</v>
+        <v>386.91287199999999</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="0"/>
-        <v>-31.425526000000005</v>
+        <v>-49.00964399999998</v>
       </c>
       <c r="K12" s="2">
         <f t="shared" si="1"/>
-        <v>-59.522855708333338</v>
+        <v>-430.08611329166683</v>
       </c>
       <c r="L12" s="2">
         <f t="shared" si="2"/>
-        <v>-66.067463124999989</v>
+        <v>-407.04188016666672</v>
       </c>
       <c r="M12" s="2">
         <f t="shared" si="3"/>
-        <v>3542.9703516750706</v>
+        <v>184974.06484633248</v>
       </c>
       <c r="N12" s="2">
         <f t="shared" si="4"/>
-        <v>4364.9096837732332</v>
+        <v>165683.09220961508</v>
       </c>
       <c r="O12" s="2">
         <f t="shared" si="5"/>
-        <v>3932.5240746050081</v>
+        <v>175063.06018781409</v>
       </c>
       <c r="P12" s="2">
         <f t="shared" si="6"/>
-        <v>987.56368437667629</v>
+        <v>2401.9452050067339</v>
       </c>
       <c r="Q12" s="2">
         <f t="shared" si="7"/>
-        <v>9504.8829285273678</v>
+        <v>207982.99269473978</v>
       </c>
       <c r="R12" s="2">
         <f t="shared" si="8"/>
-        <v>31.425526000000005</v>
+        <v>49.00964399999998</v>
       </c>
       <c r="S12">
         <v>13.139711999999999</v>
@@ -8315,7 +8315,7 @@
       </c>
       <c r="B13" s="2">
         <f>R2</f>
-        <v>45.370367249999994</v>
+        <v>117.05275720833329</v>
       </c>
       <c r="D13">
         <v>9</v>
@@ -8330,46 +8330,46 @@
         <v>31</v>
       </c>
       <c r="H13">
-        <v>47.509017999999998</v>
+        <v>543.51409899999999</v>
       </c>
       <c r="I13">
-        <v>17.277432999999998</v>
+        <v>432.39080799999999</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="0"/>
-        <v>-30.231584999999999</v>
+        <v>-111.12329099999999</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" si="1"/>
-        <v>-48.732353708333335</v>
+        <v>-384.60817729166683</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" si="2"/>
-        <v>-56.470902124999995</v>
+        <v>-299.4502971666667</v>
       </c>
       <c r="M13" s="2">
         <f t="shared" si="3"/>
-        <v>2374.8422979541097</v>
+        <v>147923.45003961824</v>
       </c>
       <c r="N13" s="2">
         <f t="shared" si="4"/>
-        <v>3188.9627868113289</v>
+        <v>89670.480473204996</v>
       </c>
       <c r="O13" s="2">
         <f t="shared" si="5"/>
-        <v>2751.9599765841722</v>
+        <v>115171.03298271967</v>
       </c>
       <c r="P13" s="2">
         <f t="shared" si="6"/>
-        <v>913.94873161222495</v>
+        <v>12348.38580267068</v>
       </c>
       <c r="Q13" s="2">
         <f t="shared" si="7"/>
-        <v>7517.3212736607893</v>
+        <v>168570.67130005162</v>
       </c>
       <c r="R13" s="2">
         <f t="shared" si="8"/>
-        <v>30.231584999999999</v>
+        <v>111.12329099999999</v>
       </c>
       <c r="S13">
         <v>12.061854</v>
@@ -8418,46 +8418,46 @@
         <v>30</v>
       </c>
       <c r="H14">
-        <v>33.267887000000002</v>
+        <v>373.34747299999998</v>
       </c>
       <c r="I14">
-        <v>9.1697410000000001</v>
+        <v>381.75524899999999</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="0"/>
-        <v>-24.098146</v>
+        <v>8.4077760000000126</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="1"/>
-        <v>-56.840045708333335</v>
+        <v>-435.24373629166683</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" si="2"/>
-        <v>-70.712033124999991</v>
+        <v>-469.61692316666671</v>
       </c>
       <c r="M14" s="2">
         <f t="shared" si="3"/>
-        <v>3230.7907961254227</v>
+        <v>189437.10998113002</v>
       </c>
       <c r="N14" s="2">
         <f t="shared" si="4"/>
-        <v>5000.1916286710957</v>
+        <v>220540.05452452693</v>
       </c>
       <c r="O14" s="2">
         <f t="shared" si="5"/>
-        <v>4019.2751949541803</v>
+        <v>204397.82426485664</v>
       </c>
       <c r="P14" s="2">
         <f t="shared" si="6"/>
-        <v>580.72064063731602</v>
+        <v>70.690697266176215</v>
       </c>
       <c r="Q14" s="2">
         <f t="shared" si="7"/>
-        <v>8988.9700657145841</v>
+        <v>212713.87743020401</v>
       </c>
       <c r="R14" s="2">
         <f t="shared" si="8"/>
-        <v>24.098146</v>
+        <v>8.4077760000000126</v>
       </c>
       <c r="S14">
         <v>5.7312029999999998</v>
@@ -8495,7 +8495,7 @@
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B15" s="6">
         <f>B5</f>
-        <v>1.1747356900297576</v>
+        <v>0.35333621499876455</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -8510,46 +8510,46 @@
         <v>31</v>
       </c>
       <c r="H15">
-        <v>46.792563999999999</v>
+        <v>508.02227800000003</v>
       </c>
       <c r="I15">
-        <v>48.831223000000001</v>
+        <v>536.34008800000004</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="0"/>
-        <v>2.0386590000000027</v>
+        <v>28.317810000000009</v>
       </c>
       <c r="K15" s="2">
         <f t="shared" si="1"/>
-        <v>-17.178563708333336</v>
+        <v>-280.65889729166679</v>
       </c>
       <c r="L15" s="2">
         <f t="shared" si="2"/>
-        <v>-57.187356124999994</v>
+        <v>-334.94211816666666</v>
       </c>
       <c r="M15" s="2">
         <f t="shared" si="3"/>
-        <v>295.10305108126715</v>
+        <v>78769.416628974373</v>
       </c>
       <c r="N15" s="2">
         <f t="shared" si="4"/>
-        <v>3270.3937005675743</v>
+        <v>112186.22252197329</v>
       </c>
       <c r="O15" s="2">
         <f t="shared" si="5"/>
-        <v>982.39664050445901</v>
+        <v>94004.485541191825</v>
       </c>
       <c r="P15" s="2">
         <f t="shared" si="6"/>
-        <v>4.1561305182810111</v>
+        <v>801.89836319610049</v>
       </c>
       <c r="Q15" s="2">
         <f t="shared" si="7"/>
-        <v>3041.3787945849822</v>
+        <v>94018.466358686957</v>
       </c>
       <c r="R15" s="2">
         <f t="shared" si="8"/>
-        <v>2.0386590000000027</v>
+        <v>28.317810000000009</v>
       </c>
       <c r="S15">
         <v>4.0966670000000001</v>
@@ -8598,46 +8598,46 @@
         <v>31</v>
       </c>
       <c r="H16">
-        <v>130.10072299999999</v>
+        <v>1263.4288329999999</v>
       </c>
       <c r="I16">
-        <v>137.00288399999999</v>
+        <v>1170.87085</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" ref="J16:J27" si="10">I16-H16</f>
-        <v>6.9021610000000067</v>
+        <v>-92.557982999999922</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" ref="K16:K27" si="11">I16-I$2</f>
-        <v>70.993097291666658</v>
+        <v>353.87186470833319</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" ref="L16:L27" si="12">H16-H$2</f>
-        <v>26.120802874999995</v>
+        <v>420.46443683333325</v>
       </c>
       <c r="M16" s="2">
         <f t="shared" ref="M16:M27" si="13">K16*K16</f>
-        <v>5040.019863064048</v>
+        <v>125225.29663215287</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" ref="N16:N27" si="14">L16*L16</f>
-        <v>682.29634283460803</v>
+        <v>176790.34264157209</v>
       </c>
       <c r="O16" s="2">
         <f t="shared" ref="O16:O27" si="15">K16*L16</f>
-        <v>1854.3966998413209</v>
+        <v>148790.5343057508</v>
       </c>
       <c r="P16" s="2">
         <f t="shared" ref="P16:P27" si="16">J16*J16</f>
-        <v>47.63982646992109</v>
+        <v>8566.9802170282746</v>
       </c>
       <c r="Q16" s="2">
         <f t="shared" ref="Q16:Q27" si="17">(I16-H$2)*(I16-H$2)</f>
-        <v>1090.516143089555</v>
+        <v>107522.64246555197</v>
       </c>
       <c r="R16" s="2">
         <f t="shared" ref="R16:R27" si="18">ABS(J16)</f>
-        <v>6.9021610000000067</v>
+        <v>92.557982999999922</v>
       </c>
       <c r="S16">
         <v>4.4663490000000001</v>
@@ -8665,46 +8665,46 @@
         <v>29</v>
       </c>
       <c r="H17">
-        <v>149.669693</v>
+        <v>1465.9085689999999</v>
       </c>
       <c r="I17">
-        <v>131.610962</v>
+        <v>1254.3043210000001</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="10"/>
-        <v>-18.058730999999995</v>
+        <v>-211.60424799999987</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" si="11"/>
-        <v>65.601175291666664</v>
+        <v>437.30533570833325</v>
       </c>
       <c r="L17" s="2">
         <f t="shared" si="12"/>
-        <v>45.689772875000003</v>
+        <v>622.94417283333325</v>
       </c>
       <c r="M17" s="2">
         <f t="shared" si="13"/>
-        <v>4303.514199647977</v>
+        <v>191235.95663897804</v>
       </c>
       <c r="N17" s="2">
         <f t="shared" si="14"/>
-        <v>2087.5553453690859</v>
+        <v>388059.44246700575</v>
       </c>
       <c r="O17" s="2">
         <f t="shared" si="15"/>
-        <v>2997.3027994093118</v>
+        <v>272416.81062843074</v>
       </c>
       <c r="P17" s="2">
         <f t="shared" si="16"/>
-        <v>326.11776533036078</v>
+        <v>44776.357771645446</v>
       </c>
       <c r="Q17" s="2">
         <f t="shared" si="17"/>
-        <v>763.47447509800395</v>
+        <v>169200.53376189235</v>
       </c>
       <c r="R17" s="2">
         <f t="shared" si="18"/>
-        <v>18.058730999999995</v>
+        <v>211.60424799999987</v>
       </c>
       <c r="S17">
         <v>4.6956059999999997</v>
@@ -8732,46 +8732,46 @@
         <v>31</v>
       </c>
       <c r="H18">
-        <v>111.083878</v>
+        <v>912.38482699999997</v>
       </c>
       <c r="I18">
-        <v>60.719954999999999</v>
+        <v>690.69152799999995</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="10"/>
-        <v>-50.363923</v>
+        <v>-221.69329900000002</v>
       </c>
       <c r="K18" s="2">
         <f t="shared" si="11"/>
-        <v>-5.2898317083333382</v>
+        <v>-126.30745729166688</v>
       </c>
       <c r="L18" s="2">
         <f t="shared" si="12"/>
-        <v>7.1039578750000061</v>
+        <v>69.420430833333285</v>
       </c>
       <c r="M18" s="2">
         <f t="shared" si="13"/>
-        <v>27.982319502488803</v>
+        <v>15953.573767486252</v>
       </c>
       <c r="N18" s="2">
         <f t="shared" si="14"/>
-        <v>50.4662174897746</v>
+        <v>4819.1962170856104</v>
       </c>
       <c r="O18" s="2">
         <f t="shared" si="15"/>
-        <v>-37.578741621839356</v>
+        <v>-8768.3181026503589</v>
       </c>
       <c r="P18" s="2">
         <f t="shared" si="16"/>
-        <v>2536.524739949929</v>
+        <v>49147.918821503408</v>
       </c>
       <c r="Q18" s="2">
         <f t="shared" si="17"/>
-        <v>1871.4245826162157</v>
+        <v>23187.026379703068</v>
       </c>
       <c r="R18" s="2">
         <f t="shared" si="18"/>
-        <v>50.363923</v>
+        <v>221.69329900000002</v>
       </c>
       <c r="S18">
         <v>5.3733880000000003</v>
@@ -8799,46 +8799,46 @@
         <v>30</v>
       </c>
       <c r="H19">
-        <v>111.655807</v>
+        <v>1197.2650149999999</v>
       </c>
       <c r="I19">
-        <v>148.37773100000001</v>
+        <v>1226.988159</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="10"/>
-        <v>36.721924000000016</v>
+        <v>29.723144000000048</v>
       </c>
       <c r="K19" s="2">
         <f t="shared" si="11"/>
-        <v>82.367944291666674</v>
+        <v>409.98917370833317</v>
       </c>
       <c r="L19" s="2">
         <f t="shared" si="12"/>
-        <v>7.6758868750000033</v>
+        <v>354.30061883333326</v>
       </c>
       <c r="M19" s="2">
         <f t="shared" si="13"/>
-        <v>6784.478246835105</v>
+        <v>168091.1225580418</v>
       </c>
       <c r="N19" s="2">
         <f t="shared" si="14"/>
-        <v>58.91923931779732</v>
+        <v>125528.9285056829</v>
       </c>
       <c r="O19" s="2">
         <f t="shared" si="15"/>
-        <v>632.24702250913572</v>
+        <v>145259.41795982941</v>
       </c>
       <c r="P19" s="2">
         <f t="shared" si="16"/>
-        <v>1348.4997022617772</v>
+        <v>883.46528924473887</v>
       </c>
       <c r="Q19" s="2">
         <f t="shared" si="17"/>
-        <v>1971.1656104922699</v>
+        <v>147474.25042067224</v>
       </c>
       <c r="R19" s="2">
         <f t="shared" si="18"/>
-        <v>36.721924000000016</v>
+        <v>29.723144000000048</v>
       </c>
       <c r="S19">
         <v>6.4953919999999998</v>
@@ -8866,46 +8866,46 @@
         <v>31</v>
       </c>
       <c r="H20">
-        <v>83.535933999999997</v>
+        <v>999.23718299999996</v>
       </c>
       <c r="I20">
-        <v>104.30669399999999</v>
+        <v>1157.6922609999999</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="10"/>
-        <v>20.770759999999996</v>
+        <v>158.45507799999996</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" si="11"/>
-        <v>38.296907291666656</v>
+        <v>340.69327570833309</v>
       </c>
       <c r="L20" s="2">
         <f t="shared" si="12"/>
-        <v>-20.443986124999995</v>
+        <v>156.27278683333327</v>
       </c>
       <c r="M20" s="2">
         <f t="shared" si="13"/>
-        <v>1466.6531081065107</v>
+        <v>116071.90811287427</v>
       </c>
       <c r="N20" s="2">
         <f t="shared" si="14"/>
-        <v>417.95656867919229</v>
+        <v>24421.18390465642</v>
       </c>
       <c r="O20" s="2">
         <f t="shared" si="15"/>
-        <v>-782.94144130124425</v>
+        <v>53241.087650318375</v>
       </c>
       <c r="P20" s="2">
         <f t="shared" si="16"/>
-        <v>431.42447097759981</v>
+        <v>25108.01174398607</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" si="17"/>
-        <v>0.10678116538251606</v>
+        <v>99053.628902548866</v>
       </c>
       <c r="R20" s="2">
         <f t="shared" si="18"/>
-        <v>20.770759999999996</v>
+        <v>158.45507799999996</v>
       </c>
       <c r="S20">
         <v>9.6104040000000008</v>
@@ -8933,46 +8933,46 @@
         <v>30</v>
       </c>
       <c r="H21">
-        <v>80.034828000000005</v>
+        <v>679.75945999999999</v>
       </c>
       <c r="I21">
-        <v>57.712505</v>
+        <v>827.918274</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="10"/>
-        <v>-22.322323000000004</v>
+        <v>148.15881400000001</v>
       </c>
       <c r="K21" s="2">
         <f t="shared" si="11"/>
-        <v>-8.2972817083333368</v>
+        <v>10.91928870833317</v>
       </c>
       <c r="L21" s="2">
         <f t="shared" si="12"/>
-        <v>-23.945092124999988</v>
+        <v>-163.2049361666667</v>
       </c>
       <c r="M21" s="2">
         <f t="shared" si="13"/>
-        <v>68.844883747442978</v>
+        <v>119.23086589593227</v>
       </c>
       <c r="N21" s="2">
         <f t="shared" si="14"/>
-        <v>573.36743687473643</v>
+        <v>26635.851189165751</v>
       </c>
       <c r="O21" s="2">
         <f t="shared" si="15"/>
-        <v>198.67917489311904</v>
+        <v>-1782.0818166289193</v>
       </c>
       <c r="P21" s="2">
         <f t="shared" si="16"/>
-        <v>498.28610411632917</v>
+        <v>21951.034165886598</v>
       </c>
       <c r="Q21" s="2">
         <f t="shared" si="17"/>
-        <v>2140.6737023490782</v>
+        <v>226.38579225425877</v>
       </c>
       <c r="R21" s="2">
         <f t="shared" si="18"/>
-        <v>22.322323000000004</v>
+        <v>148.15881400000001</v>
       </c>
       <c r="S21">
         <v>10.771552</v>
@@ -9000,46 +9000,46 @@
         <v>31</v>
       </c>
       <c r="H22">
-        <v>37.069251999999999</v>
+        <v>423.25503500000002</v>
       </c>
       <c r="I22">
-        <v>13.518675</v>
+        <v>526.04125999999997</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" si="10"/>
-        <v>-23.550576999999997</v>
+        <v>102.78622499999994</v>
       </c>
       <c r="K22" s="2">
         <f t="shared" si="11"/>
-        <v>-52.491111708333335</v>
+        <v>-290.95772529166686</v>
       </c>
       <c r="L22" s="2">
         <f t="shared" si="12"/>
-        <v>-66.910668125000001</v>
+        <v>-419.70936116666667</v>
       </c>
       <c r="M22" s="2">
         <f t="shared" si="13"/>
-        <v>2755.3168083767291</v>
+        <v>84656.397906901082</v>
       </c>
       <c r="N22" s="2">
         <f t="shared" si="14"/>
-        <v>4477.0375089338913</v>
+        <v>176155.94785093144</v>
       </c>
       <c r="O22" s="2">
         <f t="shared" si="15"/>
-        <v>3512.2153550285934</v>
+        <v>122117.68100867199</v>
       </c>
       <c r="P22" s="2">
         <f t="shared" si="16"/>
-        <v>554.62967703292884</v>
+        <v>10565.008049750613</v>
       </c>
       <c r="Q22" s="2">
         <f t="shared" si="17"/>
-        <v>8183.2368695653349</v>
+        <v>100440.27423771558</v>
       </c>
       <c r="R22" s="2">
         <f t="shared" si="18"/>
-        <v>23.550576999999997</v>
+        <v>102.78622499999994</v>
       </c>
       <c r="S22">
         <v>13.215975</v>
@@ -9067,46 +9067,46 @@
         <v>31</v>
       </c>
       <c r="H23">
-        <v>29.737268</v>
+        <v>356.11215199999998</v>
       </c>
       <c r="I23">
-        <v>4.8387399999999996</v>
+        <v>416.39163200000002</v>
       </c>
       <c r="J23" s="2">
         <f t="shared" si="10"/>
-        <v>-24.898527999999999</v>
+        <v>60.279480000000035</v>
       </c>
       <c r="K23" s="2">
         <f t="shared" si="11"/>
-        <v>-61.171046708333336</v>
+        <v>-400.60735329166681</v>
       </c>
       <c r="L23" s="2">
         <f t="shared" si="12"/>
-        <v>-74.242652124999992</v>
+        <v>-486.85224416666671</v>
       </c>
       <c r="M23" s="2">
         <f t="shared" si="13"/>
-        <v>3741.8969553930988</v>
+        <v>160486.25151135435</v>
       </c>
       <c r="N23" s="2">
         <f t="shared" si="14"/>
-        <v>5511.971394553766</v>
+        <v>237025.10765011967</v>
       </c>
       <c r="O23" s="2">
         <f t="shared" si="15"/>
-        <v>4541.5007408889178</v>
+        <v>195036.58897971667</v>
       </c>
       <c r="P23" s="2">
         <f t="shared" si="16"/>
-        <v>619.93669656678389</v>
+        <v>3633.6157090704041</v>
       </c>
       <c r="Q23" s="2">
         <f t="shared" si="17"/>
-        <v>9828.9735965776927</v>
+        <v>181964.32312879062</v>
       </c>
       <c r="R23" s="2">
         <f t="shared" si="18"/>
-        <v>24.898527999999999</v>
+        <v>60.279480000000035</v>
       </c>
       <c r="S23">
         <v>15.243527</v>
@@ -9134,46 +9134,46 @@
         <v>30</v>
       </c>
       <c r="H24">
-        <v>29.753796000000001</v>
+        <v>336.58340500000003</v>
       </c>
       <c r="I24">
-        <v>4.014062</v>
+        <v>381.95684799999998</v>
       </c>
       <c r="J24" s="2">
         <f t="shared" si="10"/>
-        <v>-25.739734000000002</v>
+        <v>45.373442999999952</v>
       </c>
       <c r="K24" s="2">
         <f t="shared" si="11"/>
-        <v>-61.995724708333334</v>
+        <v>-435.04213729166685</v>
       </c>
       <c r="L24" s="2">
         <f t="shared" si="12"/>
-        <v>-74.226124124999984</v>
+        <v>-506.38099116666666</v>
       </c>
       <c r="M24" s="2">
         <f t="shared" si="13"/>
-        <v>3843.4698821114521</v>
+        <v>189261.66121930152</v>
       </c>
       <c r="N24" s="2">
         <f t="shared" si="14"/>
-        <v>5509.5175026199049</v>
+        <v>256421.70821493573</v>
       </c>
       <c r="O24" s="2">
         <f t="shared" si="15"/>
-        <v>4601.7023574200784</v>
+        <v>220297.06868101933</v>
       </c>
       <c r="P24" s="2">
         <f t="shared" si="16"/>
-        <v>662.5339063907561</v>
+        <v>2058.7493296742446</v>
       </c>
       <c r="Q24" s="2">
         <f t="shared" si="17"/>
-        <v>9993.1727906676279</v>
+        <v>212527.95946664154</v>
       </c>
       <c r="R24" s="2">
         <f t="shared" si="18"/>
-        <v>25.739734000000002</v>
+        <v>45.373442999999952</v>
       </c>
       <c r="S24">
         <v>14.913529</v>
@@ -9201,46 +9201,46 @@
         <v>31</v>
       </c>
       <c r="H25">
-        <v>40.054530999999997</v>
+        <v>439.83184799999998</v>
       </c>
       <c r="I25">
-        <v>7.5922260000000001</v>
+        <v>418.79754600000001</v>
       </c>
       <c r="J25" s="2">
         <f t="shared" si="10"/>
-        <v>-32.462305000000001</v>
+        <v>-21.034301999999968</v>
       </c>
       <c r="K25" s="2">
         <f t="shared" si="11"/>
-        <v>-58.41756070833334</v>
+        <v>-398.20143929166682</v>
       </c>
       <c r="L25" s="2">
         <f t="shared" si="12"/>
-        <v>-63.925389124999995</v>
+        <v>-403.13254816666671</v>
       </c>
       <c r="M25" s="2">
         <f t="shared" si="13"/>
-        <v>3412.6113991118114</v>
+        <v>158564.38625395502</v>
       </c>
       <c r="N25" s="2">
         <f t="shared" si="14"/>
-        <v>4086.4553747826676</v>
+        <v>162515.85139134986</v>
       </c>
       <c r="O25" s="2">
         <f t="shared" si="15"/>
-        <v>3734.3653000135191</v>
+        <v>160527.96090528389</v>
       </c>
       <c r="P25" s="2">
         <f t="shared" si="16"/>
-        <v>1053.801245913025</v>
+        <v>442.44186062720269</v>
       </c>
       <c r="Q25" s="2">
         <f t="shared" si="17"/>
-        <v>9290.5875787345594</v>
+        <v>179917.51678031145</v>
       </c>
       <c r="R25" s="2">
         <f t="shared" si="18"/>
-        <v>32.462305000000001</v>
+        <v>21.034301999999968</v>
       </c>
       <c r="S25">
         <v>13.524543</v>
@@ -9268,46 +9268,46 @@
         <v>30</v>
       </c>
       <c r="H26">
-        <v>76.444336000000007</v>
+        <v>772.81073000000004</v>
       </c>
       <c r="I26">
-        <v>61.275429000000003</v>
+        <v>742.23394800000005</v>
       </c>
       <c r="J26" s="2">
         <f t="shared" si="10"/>
-        <v>-15.168907000000004</v>
+        <v>-30.57678199999998</v>
       </c>
       <c r="K26" s="2">
         <f t="shared" si="11"/>
-        <v>-4.7343577083333344</v>
+        <v>-74.765037291666772</v>
       </c>
       <c r="L26" s="2">
         <f t="shared" si="12"/>
-        <v>-27.535584124999986</v>
+        <v>-70.153666166666653</v>
       </c>
       <c r="M26" s="2">
         <f t="shared" si="13"/>
-        <v>22.414142910455261</v>
+        <v>5589.8108012243229</v>
       </c>
       <c r="N26" s="2">
         <f t="shared" si="14"/>
-        <v>758.20839310495126</v>
+        <v>4921.536876624109</v>
       </c>
       <c r="O26" s="2">
         <f t="shared" si="15"/>
-        <v>130.36330495565468</v>
+        <v>5245.0414670979735</v>
       </c>
       <c r="P26" s="2">
         <f t="shared" si="16"/>
-        <v>230.09573957464914</v>
+        <v>934.93959747552276</v>
       </c>
       <c r="Q26" s="2">
         <f t="shared" si="17"/>
-        <v>1823.6735622452029</v>
+        <v>10146.623187857513</v>
       </c>
       <c r="R26" s="2">
         <f t="shared" si="18"/>
-        <v>15.168907000000004</v>
+        <v>30.57678199999998</v>
       </c>
       <c r="S26">
         <v>7.9147090000000002</v>
@@ -9335,46 +9335,46 @@
         <v>31</v>
       </c>
       <c r="H27">
-        <v>162.62640400000001</v>
+        <v>1337.5745850000001</v>
       </c>
       <c r="I27">
-        <v>148.006989</v>
+        <v>1301.7392580000001</v>
       </c>
       <c r="J27" s="2">
         <f t="shared" si="10"/>
-        <v>-14.619415000000004</v>
+        <v>-35.835327000000007</v>
       </c>
       <c r="K27" s="2">
         <f t="shared" si="11"/>
-        <v>81.997202291666667</v>
+        <v>484.74027270833324</v>
       </c>
       <c r="L27" s="2">
         <f t="shared" si="12"/>
-        <v>58.646483875000015</v>
+        <v>494.61018883333338</v>
       </c>
       <c r="M27" s="2">
         <f t="shared" si="13"/>
-        <v>6723.5411836605053</v>
+        <v>234973.13198534929</v>
       </c>
       <c r="N27" s="2">
         <f t="shared" si="14"/>
-        <v>3439.410070900637</v>
+        <v>244639.2388977457</v>
       </c>
       <c r="O27" s="2">
         <f t="shared" si="15"/>
-        <v>4808.8476019933432</v>
+        <v>239757.47781939022</v>
       </c>
       <c r="P27" s="2">
         <f t="shared" si="16"/>
-        <v>213.72729494222511</v>
+        <v>1284.1706611969294</v>
       </c>
       <c r="Q27" s="2">
         <f t="shared" si="17"/>
-        <v>1938.3827937239948</v>
+        <v>210474.37385019413</v>
       </c>
       <c r="R27" s="2">
         <f t="shared" si="18"/>
-        <v>14.619415000000004</v>
+        <v>35.835327000000007</v>
       </c>
       <c r="S27">
         <v>4.2786520000000001</v>

</xml_diff>

<commit_message>
Release CW3M_Installer_1.2.2.exe. CW3M_Script.iss - Change version to 1.2.2. Add wr_pods_McKenzie.csv and wr_pous_McKenzie.csv to DataCW3M/McKenzie.
</commit_message>
<xml_diff>
--- a/DataCW3M/SkillAssessment/Flow24monthsStatisticsCalculator.xlsx
+++ b/DataCW3M/SkillAssessment/Flow24monthsStatisticsCalculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\SkillAssessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035B4E70-32A5-4EA7-8F0B-3D5DAA4BAB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F07FBB-B170-4A48-A389-CF714C59BB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics calculator" sheetId="1" r:id="rId1"/>
@@ -220,10 +220,10 @@
     <t>Phi =</t>
   </si>
   <si>
-    <t xml:space="preserve"> USGS_14178000_flow_NO SANTIAM R BLW BOULDER CRK  NR DETROIT  OR_23780591</t>
+    <t xml:space="preserve"> USGS_14158790_flow_SMITH RIVER ABV SMITH R RESV NR BELKNAP SPRINGS_23773393</t>
   </si>
   <si>
-    <t xml:space="preserve"> Obs:..\Observations\NSantiam\USGS_14178000_flow_NO SANTIAM R BLW BOULDER CRK  NR DETROIT  OR_23780591.csv</t>
+    <t xml:space="preserve"> Obs:..\Observations\McKenzie\USGS_14158790_flow_SMITH RIVER ABV SMITH R RESV NR BELKNAP SPRINGS_23773393.csv</t>
   </si>
 </sst>
 </file>
@@ -829,6 +829,17 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>'Statistics calculator'!$J$3</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v> USGS_14158790_flow_SMITH RIVER ABV SMITH R RESV NR BELKNAP SPRINGS_23773393</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -869,11 +880,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Statistics calculator'!$H$3</c:f>
+              <c:f>'Statistics calculator'!$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> USGS_14178000_flow_NO SANTIAM R BLW BOULDER CRK  NR DETROIT  OR_23780591</c:v>
+                  <c:v> USGS_14158790_flow_SMITH RIVER ABV SMITH R RESV NR BELKNAP SPRINGS_23773393</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -892,81 +903,81 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Statistics calculator'!$H$4:$H$27</c:f>
+              <c:f>'Statistics calculator'!$J$4:$J$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>1318.969116</c:v>
+                  <c:v>148.20361299999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>654.81872599999997</c:v>
+                  <c:v>54.955750000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1309.1667480000001</c:v>
+                  <c:v>144.288544</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2291.9421390000002</c:v>
+                  <c:v>275.69091800000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1116.070923</c:v>
+                  <c:v>62.521225000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>641.40801999999996</c:v>
+                  <c:v>37.737827000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>464.63085899999999</c:v>
+                  <c:v>30.045802999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>389.180969</c:v>
+                  <c:v>28.607900999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>435.92251599999997</c:v>
+                  <c:v>38.416916000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>543.51409899999999</c:v>
+                  <c:v>50.195473</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>373.34747299999998</c:v>
+                  <c:v>34.504691999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>508.02227800000003</c:v>
+                  <c:v>50.224186000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1263.4288329999999</c:v>
+                  <c:v>141.38772599999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1465.9085689999999</c:v>
+                  <c:v>171.355637</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>912.38482699999997</c:v>
+                  <c:v>115.339249</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1197.2650149999999</c:v>
+                  <c:v>103.370659</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>999.23718299999996</c:v>
+                  <c:v>86.076751999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>679.75945999999999</c:v>
+                  <c:v>85.735054000000005</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>423.25503500000002</c:v>
+                  <c:v>38.052138999999997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>356.11215199999998</c:v>
+                  <c:v>29.898626</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>336.58340500000003</c:v>
+                  <c:v>29.81213</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>439.83184799999998</c:v>
+                  <c:v>40.966869000000003</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>772.81073000000004</c:v>
+                  <c:v>86.169539999999998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1337.5745850000001</c:v>
+                  <c:v>174.08557099999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -983,11 +994,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Statistics calculator'!$I$3</c:f>
+              <c:f>'Statistics calculator'!$K$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> Obs:..\Observations\NSantiam\USGS_14178000_flow_NO SANTIAM R BLW BOULDER CRK  NR DETROIT  OR_23780591.csv</c:v>
+                  <c:v> Obs:..\Observations\McKenzie\USGS_14158790_flow_SMITH RIVER ABV SMITH R RESV NR BELKNAP SPRINGS_23773393.csv</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1006,81 +1017,81 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Statistics calculator'!$I$4:$I$27</c:f>
+              <c:f>'Statistics calculator'!$K$4:$K$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>1057.9149170000001</c:v>
+                  <c:v>110.897835</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>726.88659700000005</c:v>
+                  <c:v>46.155521</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>751.378784</c:v>
+                  <c:v>48.151909000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2731.420654</c:v>
+                  <c:v>319.90457199999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1012.70343</c:v>
+                  <c:v>70.348693999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>639.75982699999997</c:v>
+                  <c:v>18.041027</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>461.15029900000002</c:v>
+                  <c:v>6.6241539999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>373.73623700000002</c:v>
+                  <c:v>3.368989</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>386.91287199999999</c:v>
+                  <c:v>6.4869310000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>432.39080799999999</c:v>
+                  <c:v>17.277432999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>381.75524899999999</c:v>
+                  <c:v>9.1697410000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>536.34008800000004</c:v>
+                  <c:v>48.831223000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1170.87085</c:v>
+                  <c:v>137.00288399999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1254.3043210000001</c:v>
+                  <c:v>131.610962</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>690.69152799999995</c:v>
+                  <c:v>60.719954999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1226.988159</c:v>
+                  <c:v>148.37773100000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1157.6922609999999</c:v>
+                  <c:v>104.30669399999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>827.918274</c:v>
+                  <c:v>57.712505</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>526.04125999999997</c:v>
+                  <c:v>13.518675</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>416.39163200000002</c:v>
+                  <c:v>4.8387399999999996</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>381.95684799999998</c:v>
+                  <c:v>4.014062</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>418.79754600000001</c:v>
+                  <c:v>7.5922260000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>742.23394800000005</c:v>
+                  <c:v>61.275429000000003</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1301.7392580000001</c:v>
+                  <c:v>148.006989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6765,13 +6776,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>2290762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
@@ -7258,10 +7269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD3182"/>
+  <dimension ref="A1:AF3182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I3"/>
+      <selection activeCell="H3" sqref="H3:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7277,10 +7288,10 @@
     <col min="19" max="22" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="H1">
-        <f>AVERAGE(H4:H15)</f>
-        <v>837.24948883333343</v>
+        <f>AVERAGE(J4:J15)</f>
+        <v>79.616070666666658</v>
       </c>
       <c r="I1"/>
       <c r="J1"/>
@@ -7288,8 +7299,8 @@
         <v>60</v>
       </c>
       <c r="P1" s="11">
-        <f>SUM(P4:P27)</f>
-        <v>773525.67325483949</v>
+        <f>SUM(R4:R27)</f>
+        <v>29082.464728201539</v>
       </c>
       <c r="S1" t="s">
         <v>33</v>
@@ -7302,13 +7313,13 @@
       </c>
       <c r="V1"/>
     </row>
-    <row r="2" spans="1:30" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="14">
         <f>H2-I2</f>
-        <v>25.965410874999861</v>
+        <v>19.725329958333333</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -7317,12 +7328,12 @@
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2">
-        <f>AVERAGE(H4:H27)</f>
-        <v>842.96439616666669</v>
+        <f>AVERAGE(J4:J27)</f>
+        <v>85.73511666666667</v>
       </c>
       <c r="I2">
-        <f>AVERAGE(I4:I27)</f>
-        <v>816.99898529166683</v>
+        <f>AVERAGE(K4:K27)</f>
+        <v>66.009786708333337</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -7331,36 +7342,36 @@
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4">
-        <f>AVERAGE(P4:P27)</f>
-        <v>32230.236385618311</v>
+        <f>AVERAGE(R4:R27)</f>
+        <v>1211.7693636750641</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4">
-        <f>AVERAGE(R4:R27)</f>
-        <v>117.05275720833329</v>
+        <f>AVERAGE(T4:T27)</f>
+        <v>29.331841374999996</v>
       </c>
       <c r="S2">
-        <f>AVERAGE(S4:S27)</f>
+        <f>AVERAGE(U4:U27)</f>
         <v>8.6327376666666655</v>
       </c>
       <c r="T2">
-        <f>AVERAGE(T4:T27)</f>
+        <f>AVERAGE(V4:V27)</f>
         <v>9.8286382083333326</v>
       </c>
       <c r="U2"/>
       <c r="V2"/>
     </row>
-    <row r="3" spans="1:30" s="3" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" s="3" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="9">
         <f>(I2-H2)/H2</f>
-        <v>-3.0802500073640254E-2</v>
+        <v>-0.23007293539967189</v>
       </c>
       <c r="C3" s="16" t="str">
         <f>IF(ABS(B3)&lt;5%,"VG",IF(ABS(B3)&lt;10%,"G",IF(ABS(B3)&lt;15%,"S","NS")))</f>
-        <v>VG</v>
+        <v>NS</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>0</v>
@@ -7374,81 +7385,81 @@
       <c r="G3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="10">
-        <f>1-SUM(P4:P27)/SUM(M4:M27)</f>
-        <v>0.87482661896324188</v>
+        <f>1-SUM(R4:R27)/SUM(O4:O27)</f>
+        <v>0.76658475430375117</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>IF(B4&gt;0.8,"VG",IF(B4&gt;0.7,"G",IF(B4&gt;0.45,"S","NS")))</f>
-        <v>VG</v>
+        <v>G</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -7462,88 +7473,89 @@
       <c r="G4">
         <v>31</v>
       </c>
-      <c r="H4">
-        <v>1318.969116</v>
-      </c>
-      <c r="I4">
-        <v>1057.9149170000001</v>
-      </c>
-      <c r="J4" s="2">
-        <f>I4-H4</f>
-        <v>-261.05419899999993</v>
-      </c>
-      <c r="K4" s="2">
-        <f>I4-I$2</f>
-        <v>240.91593170833323</v>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4">
+        <v>148.20361299999999</v>
+      </c>
+      <c r="K4">
+        <v>110.897835</v>
       </c>
       <c r="L4" s="2">
-        <f>H4-H$2</f>
-        <v>476.0047198333333</v>
+        <f>K4-J4</f>
+        <v>-37.305777999999989</v>
       </c>
       <c r="M4" s="2">
-        <f>K4*K4</f>
-        <v>58040.486150894285</v>
+        <f>K4-I$2</f>
+        <v>44.888048291666664</v>
       </c>
       <c r="N4" s="2">
+        <f>J4-H$2</f>
+        <v>62.46849633333332</v>
+      </c>
+      <c r="O4" s="2">
+        <f>M4*M4</f>
+        <v>2014.9368794349984</v>
+      </c>
+      <c r="P4" s="2">
+        <f>N4*N4</f>
+        <v>3902.3130341476785</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>M4*N4</f>
+        <v>2804.0888801184678</v>
+      </c>
+      <c r="R4" s="2">
         <f>L4*L4</f>
-        <v>226580.49330361013</v>
-      </c>
-      <c r="O4" s="2">
-        <f>K4*L4</f>
-        <v>114677.12057621162</v>
-      </c>
-      <c r="P4" s="2">
-        <f>J4*J4</f>
-        <v>68149.294815531568</v>
-      </c>
-      <c r="Q4" s="2">
-        <f>(I4-H$2)*(I4-H$2)</f>
-        <v>46203.72640652128</v>
-      </c>
-      <c r="R4" s="2">
-        <f>ABS(J4)</f>
-        <v>261.05419899999993</v>
-      </c>
-      <c r="S4">
+        <v>1391.7210721852832</v>
+      </c>
+      <c r="S4" s="2">
+        <f>(K4-H$2)*(K4-H$2)</f>
+        <v>633.16239392266925</v>
+      </c>
+      <c r="T4" s="2">
+        <f>ABS(L4)</f>
+        <v>37.305777999999989</v>
+      </c>
+      <c r="U4">
         <v>5.1376660000000003</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <v>5.8672199999999997</v>
       </c>
-      <c r="U4">
-        <f>T4-S4</f>
+      <c r="W4">
+        <f>V4-U4</f>
         <v>0.72955399999999937</v>
       </c>
-      <c r="V4"/>
-      <c r="W4">
+      <c r="Y4">
         <v>5.224564</v>
       </c>
-      <c r="X4">
+      <c r="Z4">
         <v>6.5884280000000004</v>
       </c>
-      <c r="Y4">
+      <c r="AA4">
         <v>6.5884280000000004</v>
       </c>
-      <c r="Z4">
+      <c r="AB4">
         <v>6.5872460000000004</v>
       </c>
-      <c r="AA4">
+      <c r="AC4">
         <v>5.224564</v>
       </c>
-      <c r="AC4">
+      <c r="AE4">
         <v>6.0271819999999998</v>
       </c>
-      <c r="AD4">
+      <c r="AF4">
         <v>5.995069</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="13">
-        <f>SQRT(SUM(P4:P27))/SQRT(SUM(Q4:Q27))</f>
-        <v>0.35333621499876455</v>
+        <f>SQRT(SUM(R4:R27))/SQRT(SUM(S4:S27))</f>
+        <v>0.46598395134272419</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>IF(B5&lt;=0.5,"VG",IF(B5&lt;=0.6,"G",IF(B5&lt;=0.7,"S","NS")))</f>
@@ -7561,92 +7573,93 @@
       <c r="G5">
         <v>28</v>
       </c>
-      <c r="H5">
-        <v>654.81872599999997</v>
-      </c>
-      <c r="I5">
-        <v>726.88659700000005</v>
-      </c>
-      <c r="J5" s="2">
-        <f t="shared" ref="J5:J15" si="0">I5-H5</f>
-        <v>72.067871000000082</v>
-      </c>
-      <c r="K5" s="2">
-        <f t="shared" ref="K5:K15" si="1">I5-I$2</f>
-        <v>-90.112388291666775</v>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5">
+        <v>54.955750000000002</v>
+      </c>
+      <c r="K5">
+        <v>46.155521</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" ref="L5:L15" si="2">H5-H$2</f>
-        <v>-188.14567016666672</v>
+        <f t="shared" ref="L5:L15" si="0">K5-J5</f>
+        <v>-8.8002290000000016</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" ref="M5:M15" si="3">K5*K5</f>
-        <v>8120.2425236281233</v>
+        <f>K5-I$2</f>
+        <v>-19.854265708333337</v>
       </c>
       <c r="N5" s="2">
-        <f t="shared" ref="N5:N15" si="4">L5*L5</f>
-        <v>35398.793202464141</v>
+        <f>J5-H$2</f>
+        <v>-30.779366666666668</v>
       </c>
       <c r="O5" s="2">
-        <f t="shared" ref="O5:O15" si="5">K5*L5</f>
-        <v>16954.255685454536</v>
+        <f t="shared" ref="O5:O15" si="1">M5*M5</f>
+        <v>394.19186681710107</v>
       </c>
       <c r="P5" s="2">
-        <f t="shared" ref="P5:P15" si="6">J5*J5</f>
-        <v>5193.778030472653</v>
+        <f t="shared" ref="P5:P15" si="2">N5*N5</f>
+        <v>947.36941240111116</v>
       </c>
       <c r="Q5" s="2">
-        <f t="shared" ref="Q5:Q15" si="7">(I5-H$2)*(I5-H$2)</f>
-        <v>13474.055459376994</v>
+        <f t="shared" ref="Q5:Q15" si="3">M5*N5</f>
+        <v>611.10172413421822</v>
       </c>
       <c r="R5" s="2">
-        <f t="shared" ref="R5:R15" si="8">ABS(J5)</f>
-        <v>72.067871000000082</v>
-      </c>
-      <c r="S5">
+        <f t="shared" ref="R5:R15" si="4">L5*L5</f>
+        <v>77.444030452441027</v>
+      </c>
+      <c r="S5" s="2">
+        <f>(K5-H$2)*(K5-H$2)</f>
+        <v>1566.5443931368191</v>
+      </c>
+      <c r="T5" s="2">
+        <f t="shared" ref="T5:T15" si="5">ABS(L5)</f>
+        <v>8.8002290000000016</v>
+      </c>
+      <c r="U5">
         <v>5.2818040000000002</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>5.7384250000000003</v>
       </c>
-      <c r="U5">
-        <f t="shared" ref="U5:U15" si="9">T5-S5</f>
+      <c r="W5">
+        <f t="shared" ref="W5:W15" si="6">V5-U5</f>
         <v>0.45662100000000017</v>
       </c>
-      <c r="V5"/>
-      <c r="W5">
+      <c r="Y5">
         <v>5.8026419999999996</v>
       </c>
-      <c r="X5">
+      <c r="Z5">
         <v>5.7353670000000001</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <v>5.7353670000000001</v>
       </c>
-      <c r="Z5">
+      <c r="AB5">
         <v>6.1014759999999999</v>
       </c>
-      <c r="AA5">
+      <c r="AC5">
         <v>5.8026419999999996</v>
       </c>
-      <c r="AC5">
+      <c r="AE5">
         <v>6.0917500000000002</v>
       </c>
-      <c r="AD5">
+      <c r="AF5">
         <v>5.7064260000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="10">
         <f>B12*B12</f>
-        <v>0.87745510124463066</v>
+        <v>0.84582789952022486</v>
       </c>
       <c r="C6" s="7" t="str">
         <f>IF(B6&gt;0.85,"VG",IF(B6&gt;0.75,"G",IF(B6&gt;0.6,"S","NS")))</f>
-        <v>VG</v>
+        <v>G</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -7660,88 +7673,89 @@
       <c r="G6">
         <v>31</v>
       </c>
-      <c r="H6">
-        <v>1309.1667480000001</v>
-      </c>
-      <c r="I6">
-        <v>751.378784</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6">
+        <v>144.288544</v>
+      </c>
+      <c r="K6">
+        <v>48.151909000000003</v>
+      </c>
+      <c r="L6" s="2">
         <f t="shared" si="0"/>
-        <v>-557.7879640000001</v>
-      </c>
-      <c r="K6" s="2">
+        <v>-96.136634999999998</v>
+      </c>
+      <c r="M6" s="2">
+        <f>K6-I$2</f>
+        <v>-17.857877708333334</v>
+      </c>
+      <c r="N6" s="2">
+        <f>J6-H$2</f>
+        <v>58.553427333333332</v>
+      </c>
+      <c r="O6" s="2">
         <f t="shared" si="1"/>
-        <v>-65.620201291666831</v>
-      </c>
-      <c r="L6" s="2">
+        <v>318.90379624578861</v>
+      </c>
+      <c r="P6" s="2">
         <f t="shared" si="2"/>
-        <v>466.20235183333341</v>
-      </c>
-      <c r="M6" s="2">
+        <v>3428.503852479947</v>
+      </c>
+      <c r="Q6" s="2">
         <f t="shared" si="3"/>
-        <v>4306.010817558873</v>
-      </c>
-      <c r="N6" s="2">
+        <v>-1045.6399447224489</v>
+      </c>
+      <c r="R6" s="2">
         <f t="shared" si="4"/>
-        <v>217344.6328549312</v>
-      </c>
-      <c r="O6" s="2">
+        <v>9242.2525891232253</v>
+      </c>
+      <c r="S6" s="2">
+        <f>(K6-H$2)*(K6-H$2)</f>
+        <v>1412.4974985157921</v>
+      </c>
+      <c r="T6" s="2">
         <f t="shared" si="5"/>
-        <v>-30592.292169951819</v>
-      </c>
-      <c r="P6" s="2">
+        <v>96.136634999999998</v>
+      </c>
+      <c r="U6">
+        <v>5.855613</v>
+      </c>
+      <c r="V6">
+        <v>6.4123729999999997</v>
+      </c>
+      <c r="W6">
         <f t="shared" si="6"/>
-        <v>311127.4127832654</v>
-      </c>
-      <c r="Q6" s="2">
-        <f t="shared" si="7"/>
-        <v>8387.9243559430852</v>
-      </c>
-      <c r="R6" s="2">
-        <f t="shared" si="8"/>
-        <v>557.7879640000001</v>
-      </c>
-      <c r="S6">
-        <v>5.855613</v>
-      </c>
-      <c r="T6">
-        <v>6.4123729999999997</v>
-      </c>
-      <c r="U6">
-        <f t="shared" si="9"/>
         <v>0.5567599999999997</v>
       </c>
-      <c r="V6"/>
-      <c r="W6">
+      <c r="Y6">
         <v>5.923997</v>
       </c>
-      <c r="X6">
+      <c r="Z6">
         <v>5.882441</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <v>5.882441</v>
       </c>
-      <c r="Z6">
+      <c r="AB6">
         <v>7.3270049999999998</v>
       </c>
-      <c r="AA6">
+      <c r="AC6">
         <v>5.923997</v>
       </c>
-      <c r="AC6">
+      <c r="AE6">
         <v>6.2149340000000004</v>
       </c>
-      <c r="AD6">
+      <c r="AF6">
         <v>5.4635199999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="1">
         <f>H2</f>
-        <v>842.96439616666669</v>
+        <v>85.73511666666667</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7">
@@ -7756,88 +7770,89 @@
       <c r="G7">
         <v>30</v>
       </c>
-      <c r="H7">
-        <v>2291.9421390000002</v>
-      </c>
-      <c r="I7">
-        <v>2731.420654</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7">
+        <v>275.69091800000001</v>
+      </c>
+      <c r="K7">
+        <v>319.90457199999997</v>
+      </c>
+      <c r="L7" s="2">
         <f t="shared" si="0"/>
-        <v>439.47851499999979</v>
-      </c>
-      <c r="K7" s="2">
+        <v>44.213653999999963</v>
+      </c>
+      <c r="M7" s="2">
+        <f>K7-I$2</f>
+        <v>253.89478529166664</v>
+      </c>
+      <c r="N7" s="2">
+        <f>J7-H$2</f>
+        <v>189.95580133333334</v>
+      </c>
+      <c r="O7" s="2">
         <f t="shared" si="1"/>
-        <v>1914.4216687083331</v>
-      </c>
-      <c r="L7" s="2">
+        <v>64462.561998301499</v>
+      </c>
+      <c r="P7" s="2">
         <f t="shared" si="2"/>
-        <v>1448.9777428333337</v>
-      </c>
-      <c r="M7" s="2">
+        <v>36083.206460188805</v>
+      </c>
+      <c r="Q7" s="2">
         <f t="shared" si="3"/>
-        <v>3665010.3256199984</v>
-      </c>
-      <c r="N7" s="2">
+        <v>48228.787394433151</v>
+      </c>
+      <c r="R7" s="2">
         <f t="shared" si="4"/>
-        <v>2099536.4992263825</v>
-      </c>
-      <c r="O7" s="2">
+        <v>1954.8472000317126</v>
+      </c>
+      <c r="S7" s="2">
+        <f>(K7-H$2)*(K7-H$2)</f>
+        <v>54835.33381110998</v>
+      </c>
+      <c r="T7" s="2">
         <f t="shared" si="5"/>
-        <v>2773954.3883562246</v>
-      </c>
-      <c r="P7" s="2">
+        <v>44.213653999999963</v>
+      </c>
+      <c r="U7">
+        <v>6.2127059999999998</v>
+      </c>
+      <c r="V7">
+        <v>6.5012179999999997</v>
+      </c>
+      <c r="W7">
         <f t="shared" si="6"/>
-        <v>193141.36514660504</v>
-      </c>
-      <c r="Q7" s="2">
-        <f t="shared" si="7"/>
-        <v>3566267.0377498777</v>
-      </c>
-      <c r="R7" s="2">
-        <f t="shared" si="8"/>
-        <v>439.47851499999979</v>
-      </c>
-      <c r="S7">
-        <v>6.2127059999999998</v>
-      </c>
-      <c r="T7">
-        <v>6.5012179999999997</v>
-      </c>
-      <c r="U7">
-        <f t="shared" si="9"/>
         <v>0.28851199999999988</v>
       </c>
-      <c r="V7"/>
-      <c r="W7">
+      <c r="Y7">
         <v>7.5821870000000002</v>
       </c>
-      <c r="X7">
+      <c r="Z7">
         <v>6.2105370000000004</v>
       </c>
-      <c r="Y7">
+      <c r="AA7">
         <v>6.2105370000000004</v>
       </c>
-      <c r="Z7">
+      <c r="AB7">
         <v>8.4893850000000004</v>
       </c>
-      <c r="AA7">
+      <c r="AC7">
         <v>7.5821870000000002</v>
       </c>
-      <c r="AC7">
+      <c r="AE7">
         <v>6.6572610000000001</v>
       </c>
-      <c r="AD7">
+      <c r="AF7">
         <v>5.8469829999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="1">
-        <f>_xlfn.STDEV.P(H4:H27)</f>
-        <v>476.93214122539456</v>
+        <f>_xlfn.STDEV.P(J4:J27)</f>
+        <v>61.543028612638878</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8">
@@ -7852,88 +7867,89 @@
       <c r="G8">
         <v>31</v>
       </c>
-      <c r="H8">
-        <v>1116.070923</v>
-      </c>
-      <c r="I8">
-        <v>1012.70343</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8">
+        <v>62.521225000000001</v>
+      </c>
+      <c r="K8">
+        <v>70.348693999999995</v>
+      </c>
+      <c r="L8" s="2">
         <f t="shared" si="0"/>
-        <v>-103.36749299999997</v>
-      </c>
-      <c r="K8" s="2">
+        <v>7.8274689999999936</v>
+      </c>
+      <c r="M8" s="2">
+        <f>K8-I$2</f>
+        <v>4.3389072916666578</v>
+      </c>
+      <c r="N8" s="2">
+        <f>J8-H$2</f>
+        <v>-23.213891666666669</v>
+      </c>
+      <c r="O8" s="2">
         <f t="shared" si="1"/>
-        <v>195.7044447083332</v>
-      </c>
-      <c r="L8" s="2">
+        <v>18.826116485678092</v>
+      </c>
+      <c r="P8" s="2">
         <f t="shared" si="2"/>
-        <v>273.10652683333331</v>
-      </c>
-      <c r="M8" s="2">
+        <v>538.88476631173626</v>
+      </c>
+      <c r="Q8" s="2">
         <f t="shared" si="3"/>
-        <v>38300.229678597047</v>
-      </c>
-      <c r="N8" s="2">
+        <v>-100.72292382045987</v>
+      </c>
+      <c r="R8" s="2">
         <f t="shared" si="4"/>
-        <v>74587.174998966206</v>
-      </c>
-      <c r="O8" s="2">
+        <v>61.269270945960898</v>
+      </c>
+      <c r="S8" s="2">
+        <f>(K8-H$2)*(K8-H$2)</f>
+        <v>236.74200247731403</v>
+      </c>
+      <c r="T8" s="2">
         <f t="shared" si="5"/>
-        <v>53448.161180138995</v>
-      </c>
-      <c r="P8" s="2">
+        <v>7.8274689999999936</v>
+      </c>
+      <c r="U8">
+        <v>6.9663380000000004</v>
+      </c>
+      <c r="V8">
+        <v>7.5264199999999999</v>
+      </c>
+      <c r="W8">
         <f t="shared" si="6"/>
-        <v>10684.838609105042</v>
-      </c>
-      <c r="Q8" s="2">
-        <f t="shared" si="7"/>
-        <v>28811.339606673479</v>
-      </c>
-      <c r="R8" s="2">
-        <f t="shared" si="8"/>
-        <v>103.36749299999997</v>
-      </c>
-      <c r="S8">
-        <v>6.9663380000000004</v>
-      </c>
-      <c r="T8">
-        <v>7.5264199999999999</v>
-      </c>
-      <c r="U8">
-        <f t="shared" si="9"/>
         <v>0.56008199999999952</v>
       </c>
-      <c r="V8"/>
-      <c r="W8">
+      <c r="Y8">
         <v>9.4392139999999998</v>
       </c>
-      <c r="X8">
+      <c r="Z8">
         <v>6.5755290000000004</v>
       </c>
-      <c r="Y8">
+      <c r="AA8">
         <v>6.5755290000000004</v>
       </c>
-      <c r="Z8">
+      <c r="AB8">
         <v>9.9157399999999996</v>
       </c>
-      <c r="AA8">
+      <c r="AC8">
         <v>9.4392139999999998</v>
       </c>
-      <c r="AC8">
+      <c r="AE8">
         <v>8.2361129999999996</v>
       </c>
-      <c r="AD8">
+      <c r="AF8">
         <v>7.3546389999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="1">
         <f>I2</f>
-        <v>816.99898529166683</v>
+        <v>66.009786708333337</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9">
@@ -7948,88 +7964,89 @@
       <c r="G9">
         <v>30</v>
       </c>
-      <c r="H9">
-        <v>641.40801999999996</v>
-      </c>
-      <c r="I9">
-        <v>639.75982699999997</v>
-      </c>
-      <c r="J9" s="2">
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9">
+        <v>37.737827000000003</v>
+      </c>
+      <c r="K9">
+        <v>18.041027</v>
+      </c>
+      <c r="L9" s="2">
         <f t="shared" si="0"/>
-        <v>-1.648192999999992</v>
-      </c>
-      <c r="K9" s="2">
+        <v>-19.696800000000003</v>
+      </c>
+      <c r="M9" s="2">
+        <f>K9-I$2</f>
+        <v>-47.968759708333337</v>
+      </c>
+      <c r="N9" s="2">
+        <f>J9-H$2</f>
+        <v>-47.997289666666667</v>
+      </c>
+      <c r="O9" s="2">
         <f t="shared" si="1"/>
-        <v>-177.23915829166685</v>
-      </c>
-      <c r="L9" s="2">
+        <v>2301.0019079558238</v>
+      </c>
+      <c r="P9" s="2">
         <f t="shared" si="2"/>
-        <v>-201.55637616666672</v>
-      </c>
-      <c r="M9" s="2">
+        <v>2303.7398153459067</v>
+      </c>
+      <c r="Q9" s="2">
         <f t="shared" si="3"/>
-        <v>31413.719231938539</v>
-      </c>
-      <c r="N9" s="2">
+        <v>2302.370454671604</v>
+      </c>
+      <c r="R9" s="2">
         <f t="shared" si="4"/>
-        <v>40624.972773438858</v>
-      </c>
-      <c r="O9" s="2">
+        <v>387.96393024000014</v>
+      </c>
+      <c r="S9" s="2">
+        <f>(K9-H$2)*(K9-H$2)</f>
+        <v>4582.4897757987073</v>
+      </c>
+      <c r="T9" s="2">
         <f t="shared" si="5"/>
-        <v>35723.682460098593</v>
-      </c>
-      <c r="P9" s="2">
+        <v>19.696800000000003</v>
+      </c>
+      <c r="U9">
+        <v>8.0567130000000002</v>
+      </c>
+      <c r="V9">
+        <v>9.3709589999999992</v>
+      </c>
+      <c r="W9">
         <f t="shared" si="6"/>
-        <v>2.7165401652489738</v>
-      </c>
-      <c r="Q9" s="2">
-        <f t="shared" si="7"/>
-        <v>41292.096930210639</v>
-      </c>
-      <c r="R9" s="2">
-        <f t="shared" si="8"/>
-        <v>1.648192999999992</v>
-      </c>
-      <c r="S9">
-        <v>8.0567130000000002</v>
-      </c>
-      <c r="T9">
-        <v>9.3709589999999992</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="9"/>
         <v>1.3142459999999989</v>
       </c>
-      <c r="V9"/>
-      <c r="W9">
+      <c r="Y9">
         <v>9.8762489999999996</v>
       </c>
-      <c r="X9">
+      <c r="Z9">
         <v>6.801971</v>
       </c>
-      <c r="Y9">
+      <c r="AA9">
         <v>6.801971</v>
       </c>
-      <c r="Z9">
+      <c r="AB9">
         <v>11.143119</v>
       </c>
-      <c r="AA9">
+      <c r="AC9">
         <v>9.8762489999999996</v>
       </c>
-      <c r="AC9">
+      <c r="AE9">
         <v>11.508697</v>
       </c>
-      <c r="AD9">
+      <c r="AF9">
         <v>9.6800379999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="1">
-        <f>_xlfn.STDEV.P(I4:I27)</f>
-        <v>507.42954910553692</v>
+        <f>_xlfn.STDEV.P(K4:K27)</f>
+        <v>72.051889567013248</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -8043,88 +8060,89 @@
       <c r="G10">
         <v>31</v>
       </c>
-      <c r="H10">
-        <v>464.63085899999999</v>
-      </c>
-      <c r="I10">
-        <v>461.15029900000002</v>
-      </c>
-      <c r="J10" s="2">
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10">
+        <v>30.045802999999999</v>
+      </c>
+      <c r="K10">
+        <v>6.6241539999999999</v>
+      </c>
+      <c r="L10" s="2">
         <f t="shared" si="0"/>
-        <v>-3.4805599999999686</v>
-      </c>
-      <c r="K10" s="2">
+        <v>-23.421648999999999</v>
+      </c>
+      <c r="M10" s="2">
+        <f>K10-I$2</f>
+        <v>-59.38563270833334</v>
+      </c>
+      <c r="N10" s="2">
+        <f>J10-H$2</f>
+        <v>-55.689313666666671</v>
+      </c>
+      <c r="O10" s="2">
         <f t="shared" si="1"/>
-        <v>-355.84868629166681</v>
-      </c>
-      <c r="L10" s="2">
+        <v>3526.6533721690707</v>
+      </c>
+      <c r="P10" s="2">
         <f t="shared" si="2"/>
-        <v>-378.3335371666667</v>
-      </c>
-      <c r="M10" s="2">
+        <v>3101.2996566643874</v>
+      </c>
+      <c r="Q10" s="2">
         <f t="shared" si="3"/>
-        <v>126628.28753550509</v>
-      </c>
-      <c r="N10" s="2">
+        <v>3307.145127187835</v>
+      </c>
+      <c r="R10" s="2">
         <f t="shared" si="4"/>
-        <v>143136.26534504158</v>
-      </c>
-      <c r="O10" s="2">
+        <v>548.57364187920098</v>
+      </c>
+      <c r="S10" s="2">
+        <f>(K10-H$2)*(K10-H$2)</f>
+        <v>6258.5444140467271</v>
+      </c>
+      <c r="T10" s="2">
         <f t="shared" si="5"/>
-        <v>134629.49218083784</v>
-      </c>
-      <c r="P10" s="2">
+        <v>23.421648999999999</v>
+      </c>
+      <c r="U10">
+        <v>10.862743</v>
+      </c>
+      <c r="V10">
+        <v>12.556028</v>
+      </c>
+      <c r="W10">
         <f t="shared" si="6"/>
-        <v>12.114297913599781</v>
-      </c>
-      <c r="Q10" s="2">
-        <f t="shared" si="7"/>
-        <v>145782.00479519679</v>
-      </c>
-      <c r="R10" s="2">
-        <f t="shared" si="8"/>
-        <v>3.4805599999999686</v>
-      </c>
-      <c r="S10">
-        <v>10.862743</v>
-      </c>
-      <c r="T10">
-        <v>12.556028</v>
-      </c>
-      <c r="U10">
-        <f t="shared" si="9"/>
         <v>1.6932849999999995</v>
       </c>
-      <c r="V10"/>
-      <c r="W10">
+      <c r="Y10">
         <v>13.152755000000001</v>
       </c>
-      <c r="X10">
+      <c r="Z10">
         <v>7.1369730000000002</v>
       </c>
-      <c r="Y10">
+      <c r="AA10">
         <v>7.1369730000000002</v>
       </c>
-      <c r="Z10">
+      <c r="AB10">
         <v>13.856355000000001</v>
       </c>
-      <c r="AA10">
+      <c r="AC10">
         <v>13.152755000000001</v>
       </c>
-      <c r="AC10">
+      <c r="AE10">
         <v>16.489000000000001</v>
       </c>
-      <c r="AD10">
+      <c r="AF10">
         <v>14.584220999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="1">
         <f>SQRT(P$2)</f>
-        <v>179.52781507504153</v>
+        <v>34.810477785791221</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -8138,88 +8156,89 @@
       <c r="G11">
         <v>31</v>
       </c>
-      <c r="H11">
-        <v>389.180969</v>
-      </c>
-      <c r="I11">
-        <v>373.73623700000002</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11">
+        <v>28.607900999999998</v>
+      </c>
+      <c r="K11">
+        <v>3.368989</v>
+      </c>
+      <c r="L11" s="2">
         <f t="shared" si="0"/>
-        <v>-15.444731999999988</v>
-      </c>
-      <c r="K11" s="2">
+        <v>-25.238911999999999</v>
+      </c>
+      <c r="M11" s="2">
+        <f>K11-I$2</f>
+        <v>-62.640797708333338</v>
+      </c>
+      <c r="N11" s="2">
+        <f>J11-H$2</f>
+        <v>-57.127215666666672</v>
+      </c>
+      <c r="O11" s="2">
         <f t="shared" si="1"/>
-        <v>-443.26274829166681</v>
-      </c>
-      <c r="L11" s="2">
+        <v>3923.8695375363391</v>
+      </c>
+      <c r="P11" s="2">
         <f t="shared" si="2"/>
-        <v>-453.78342716666668</v>
-      </c>
-      <c r="M11" s="2">
+        <v>3263.518769825846</v>
+      </c>
+      <c r="Q11" s="2">
         <f t="shared" si="3"/>
-        <v>196481.86402308158</v>
-      </c>
-      <c r="N11" s="2">
+        <v>3578.4943602159979</v>
+      </c>
+      <c r="R11" s="2">
         <f t="shared" si="4"/>
-        <v>205919.39877112547</v>
-      </c>
-      <c r="O11" s="2">
+        <v>637.00267894374394</v>
+      </c>
+      <c r="S11" s="2">
+        <f>(K11-H$2)*(K11-H$2)</f>
+        <v>6784.1789868016331</v>
+      </c>
+      <c r="T11" s="2">
         <f t="shared" si="5"/>
-        <v>201145.28905510809</v>
-      </c>
-      <c r="P11" s="2">
+        <v>25.238911999999999</v>
+      </c>
+      <c r="U11">
+        <v>13.279059</v>
+      </c>
+      <c r="V11">
+        <v>15.188703</v>
+      </c>
+      <c r="W11">
         <f t="shared" si="6"/>
-        <v>238.53974655182361</v>
-      </c>
-      <c r="Q11" s="2">
-        <f t="shared" si="7"/>
-        <v>220175.06535493868</v>
-      </c>
-      <c r="R11" s="2">
-        <f t="shared" si="8"/>
-        <v>15.444731999999988</v>
-      </c>
-      <c r="S11">
-        <v>13.279059</v>
-      </c>
-      <c r="T11">
-        <v>15.188703</v>
-      </c>
-      <c r="U11">
-        <f t="shared" si="9"/>
         <v>1.9096440000000001</v>
       </c>
-      <c r="V11"/>
-      <c r="W11">
+      <c r="Y11">
         <v>13.913205</v>
       </c>
-      <c r="X11">
+      <c r="Z11">
         <v>7.4031919999999998</v>
       </c>
-      <c r="Y11">
+      <c r="AA11">
         <v>7.4031919999999998</v>
       </c>
-      <c r="Z11">
+      <c r="AB11">
         <v>16.792356000000002</v>
       </c>
-      <c r="AA11">
+      <c r="AC11">
         <v>13.913205</v>
       </c>
-      <c r="AC11">
+      <c r="AE11">
         <v>16.392616</v>
       </c>
-      <c r="AD11">
+      <c r="AF11">
         <v>15.261647999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1">
-        <f>SUM(O4:O27)/SQRT(SUM(M4:M27)*SUM(N4:N27))</f>
-        <v>0.93672573427051242</v>
+        <f>SUM(Q4:Q27)/SQRT(SUM(O4:O27)*SUM(P4:P27))</f>
+        <v>0.9196890232683137</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12">
@@ -8234,88 +8253,89 @@
       <c r="G12">
         <v>30</v>
       </c>
-      <c r="H12">
-        <v>435.92251599999997</v>
-      </c>
-      <c r="I12">
-        <v>386.91287199999999</v>
-      </c>
-      <c r="J12" s="2">
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12">
+        <v>38.416916000000001</v>
+      </c>
+      <c r="K12">
+        <v>6.4869310000000002</v>
+      </c>
+      <c r="L12" s="2">
         <f t="shared" si="0"/>
-        <v>-49.00964399999998</v>
-      </c>
-      <c r="K12" s="2">
+        <v>-31.929985000000002</v>
+      </c>
+      <c r="M12" s="2">
+        <f>K12-I$2</f>
+        <v>-59.522855708333338</v>
+      </c>
+      <c r="N12" s="2">
+        <f>J12-H$2</f>
+        <v>-47.318200666666669</v>
+      </c>
+      <c r="O12" s="2">
         <f t="shared" si="1"/>
-        <v>-430.08611329166683</v>
-      </c>
-      <c r="L12" s="2">
+        <v>3542.9703516750706</v>
+      </c>
+      <c r="P12" s="2">
         <f t="shared" si="2"/>
-        <v>-407.04188016666672</v>
-      </c>
-      <c r="M12" s="2">
+        <v>2239.0121143309339</v>
+      </c>
+      <c r="Q12" s="2">
         <f t="shared" si="3"/>
-        <v>184974.06484633248</v>
-      </c>
-      <c r="N12" s="2">
+        <v>2816.5144306599627</v>
+      </c>
+      <c r="R12" s="2">
         <f t="shared" si="4"/>
-        <v>165683.09220961508</v>
-      </c>
-      <c r="O12" s="2">
+        <v>1019.5239421002251</v>
+      </c>
+      <c r="S12" s="2">
+        <f>(K12-H$2)*(K12-H$2)</f>
+        <v>6280.2749314584726</v>
+      </c>
+      <c r="T12" s="2">
         <f t="shared" si="5"/>
-        <v>175063.06018781409</v>
-      </c>
-      <c r="P12" s="2">
+        <v>31.929985000000002</v>
+      </c>
+      <c r="U12">
+        <v>13.139711999999999</v>
+      </c>
+      <c r="V12">
+        <v>15.156300999999999</v>
+      </c>
+      <c r="W12">
         <f t="shared" si="6"/>
-        <v>2401.9452050067339</v>
-      </c>
-      <c r="Q12" s="2">
-        <f t="shared" si="7"/>
-        <v>207982.99269473978</v>
-      </c>
-      <c r="R12" s="2">
-        <f t="shared" si="8"/>
-        <v>49.00964399999998</v>
-      </c>
-      <c r="S12">
-        <v>13.139711999999999</v>
-      </c>
-      <c r="T12">
-        <v>15.156300999999999</v>
-      </c>
-      <c r="U12">
-        <f t="shared" si="9"/>
         <v>2.0165889999999997</v>
       </c>
-      <c r="V12"/>
-      <c r="W12">
+      <c r="Y12">
         <v>12.812222</v>
       </c>
-      <c r="X12">
+      <c r="Z12">
         <v>7.5716789999999996</v>
       </c>
-      <c r="Y12">
+      <c r="AA12">
         <v>7.5716789999999996</v>
       </c>
-      <c r="Z12">
+      <c r="AB12">
         <v>18.412051999999999</v>
       </c>
-      <c r="AA12">
+      <c r="AC12">
         <v>12.812222</v>
       </c>
-      <c r="AC12">
+      <c r="AE12">
         <v>12.729642999999999</v>
       </c>
-      <c r="AD12">
+      <c r="AF12">
         <v>12.806131000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="2">
         <f>R2</f>
-        <v>117.05275720833329</v>
+        <v>29.331841374999996</v>
       </c>
       <c r="D13">
         <v>9</v>
@@ -8329,82 +8349,83 @@
       <c r="G13">
         <v>31</v>
       </c>
-      <c r="H13">
-        <v>543.51409899999999</v>
-      </c>
-      <c r="I13">
-        <v>432.39080799999999</v>
-      </c>
-      <c r="J13" s="2">
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13">
+        <v>50.195473</v>
+      </c>
+      <c r="K13">
+        <v>17.277432999999998</v>
+      </c>
+      <c r="L13" s="2">
         <f t="shared" si="0"/>
-        <v>-111.12329099999999</v>
-      </c>
-      <c r="K13" s="2">
+        <v>-32.918040000000005</v>
+      </c>
+      <c r="M13" s="2">
+        <f>K13-I$2</f>
+        <v>-48.732353708333335</v>
+      </c>
+      <c r="N13" s="2">
+        <f>J13-H$2</f>
+        <v>-35.53964366666667</v>
+      </c>
+      <c r="O13" s="2">
         <f t="shared" si="1"/>
-        <v>-384.60817729166683</v>
-      </c>
-      <c r="L13" s="2">
+        <v>2374.8422979541097</v>
+      </c>
+      <c r="P13" s="2">
         <f t="shared" si="2"/>
-        <v>-299.4502971666667</v>
-      </c>
-      <c r="M13" s="2">
+        <v>1263.0662719536404</v>
+      </c>
+      <c r="Q13" s="2">
         <f t="shared" si="3"/>
-        <v>147923.45003961824</v>
-      </c>
-      <c r="N13" s="2">
+        <v>1731.9304858321289</v>
+      </c>
+      <c r="R13" s="2">
         <f t="shared" si="4"/>
-        <v>89670.480473204996</v>
-      </c>
-      <c r="O13" s="2">
+        <v>1083.5973574416003</v>
+      </c>
+      <c r="S13" s="2">
+        <f>(K13-H$2)*(K13-H$2)</f>
+        <v>4686.4544530054</v>
+      </c>
+      <c r="T13" s="2">
         <f t="shared" si="5"/>
-        <v>115171.03298271967</v>
-      </c>
-      <c r="P13" s="2">
+        <v>32.918040000000005</v>
+      </c>
+      <c r="U13">
+        <v>12.061854</v>
+      </c>
+      <c r="V13">
+        <v>14.002096</v>
+      </c>
+      <c r="W13">
         <f t="shared" si="6"/>
-        <v>12348.38580267068</v>
-      </c>
-      <c r="Q13" s="2">
-        <f t="shared" si="7"/>
-        <v>168570.67130005162</v>
-      </c>
-      <c r="R13" s="2">
-        <f t="shared" si="8"/>
-        <v>111.12329099999999</v>
-      </c>
-      <c r="S13">
-        <v>12.061854</v>
-      </c>
-      <c r="T13">
-        <v>14.002096</v>
-      </c>
-      <c r="U13">
-        <f t="shared" si="9"/>
         <v>1.9402419999999996</v>
       </c>
-      <c r="V13"/>
-      <c r="W13">
+      <c r="Y13">
         <v>9.4167349999999992</v>
       </c>
-      <c r="X13">
+      <c r="Z13">
         <v>7.5526289999999996</v>
       </c>
-      <c r="Y13">
+      <c r="AA13">
         <v>7.5526289999999996</v>
       </c>
-      <c r="Z13">
+      <c r="AB13">
         <v>18.058346</v>
       </c>
-      <c r="AA13">
+      <c r="AC13">
         <v>9.4167349999999992</v>
       </c>
-      <c r="AC13">
+      <c r="AE13">
         <v>9.5897050000000004</v>
       </c>
-      <c r="AD13">
+      <c r="AF13">
         <v>9.8069469999999992</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="D14">
         <v>10</v>
       </c>
@@ -8417,85 +8438,86 @@
       <c r="G14">
         <v>30</v>
       </c>
-      <c r="H14">
-        <v>373.34747299999998</v>
-      </c>
-      <c r="I14">
-        <v>381.75524899999999</v>
-      </c>
-      <c r="J14" s="2">
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14">
+        <v>34.504691999999999</v>
+      </c>
+      <c r="K14">
+        <v>9.1697410000000001</v>
+      </c>
+      <c r="L14" s="2">
         <f t="shared" si="0"/>
-        <v>8.4077760000000126</v>
-      </c>
-      <c r="K14" s="2">
+        <v>-25.334950999999997</v>
+      </c>
+      <c r="M14" s="2">
+        <f>K14-I$2</f>
+        <v>-56.840045708333335</v>
+      </c>
+      <c r="N14" s="2">
+        <f>J14-H$2</f>
+        <v>-51.230424666666671</v>
+      </c>
+      <c r="O14" s="2">
         <f t="shared" si="1"/>
-        <v>-435.24373629166683</v>
-      </c>
-      <c r="L14" s="2">
+        <v>3230.7907961254227</v>
+      </c>
+      <c r="P14" s="2">
         <f t="shared" si="2"/>
-        <v>-469.61692316666671</v>
-      </c>
-      <c r="M14" s="2">
+        <v>2624.556411527009</v>
+      </c>
+      <c r="Q14" s="2">
         <f t="shared" si="3"/>
-        <v>189437.10998113002</v>
-      </c>
-      <c r="N14" s="2">
+        <v>2911.939679710661</v>
+      </c>
+      <c r="R14" s="2">
         <f t="shared" si="4"/>
-        <v>220540.05452452693</v>
-      </c>
-      <c r="O14" s="2">
+        <v>641.85974217240084</v>
+      </c>
+      <c r="S14" s="2">
+        <f>(K14-H$2)*(K14-H$2)</f>
+        <v>5862.2567509777928</v>
+      </c>
+      <c r="T14" s="2">
         <f t="shared" si="5"/>
-        <v>204397.82426485664</v>
-      </c>
-      <c r="P14" s="2">
+        <v>25.334950999999997</v>
+      </c>
+      <c r="U14">
+        <v>5.7312029999999998</v>
+      </c>
+      <c r="V14">
+        <v>6.2288560000000004</v>
+      </c>
+      <c r="W14">
         <f t="shared" si="6"/>
-        <v>70.690697266176215</v>
-      </c>
-      <c r="Q14" s="2">
-        <f t="shared" si="7"/>
-        <v>212713.87743020401</v>
-      </c>
-      <c r="R14" s="2">
-        <f t="shared" si="8"/>
-        <v>8.4077760000000126</v>
-      </c>
-      <c r="S14">
-        <v>5.7312029999999998</v>
-      </c>
-      <c r="T14">
-        <v>6.2288560000000004</v>
-      </c>
-      <c r="U14">
-        <f t="shared" si="9"/>
         <v>0.49765300000000057</v>
       </c>
-      <c r="V14"/>
-      <c r="W14">
+      <c r="Y14">
         <v>7.0914609999999998</v>
       </c>
-      <c r="X14">
+      <c r="Z14">
         <v>6.8328519999999999</v>
       </c>
-      <c r="Y14">
+      <c r="AA14">
         <v>6.8328519999999999</v>
       </c>
-      <c r="Z14">
+      <c r="AB14">
         <v>13.442185</v>
       </c>
-      <c r="AA14">
+      <c r="AC14">
         <v>7.0914609999999998</v>
       </c>
-      <c r="AC14">
+      <c r="AE14">
         <v>5.0972689999999998</v>
       </c>
-      <c r="AD14">
+      <c r="AF14">
         <v>6.3599959999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B15" s="6">
         <f>B5</f>
-        <v>0.35333621499876455</v>
+        <v>0.46598395134272419</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -8509,82 +8531,83 @@
       <c r="G15">
         <v>31</v>
       </c>
-      <c r="H15">
-        <v>508.02227800000003</v>
-      </c>
-      <c r="I15">
-        <v>536.34008800000004</v>
-      </c>
-      <c r="J15" s="2">
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15">
+        <v>50.224186000000003</v>
+      </c>
+      <c r="K15">
+        <v>48.831223000000001</v>
+      </c>
+      <c r="L15" s="2">
         <f t="shared" si="0"/>
-        <v>28.317810000000009</v>
-      </c>
-      <c r="K15" s="2">
+        <v>-1.3929630000000017</v>
+      </c>
+      <c r="M15" s="2">
+        <f>K15-I$2</f>
+        <v>-17.178563708333336</v>
+      </c>
+      <c r="N15" s="2">
+        <f>J15-H$2</f>
+        <v>-35.510930666666667</v>
+      </c>
+      <c r="O15" s="2">
         <f t="shared" si="1"/>
-        <v>-280.65889729166679</v>
-      </c>
-      <c r="L15" s="2">
+        <v>295.10305108126715</v>
+      </c>
+      <c r="P15" s="2">
         <f t="shared" si="2"/>
-        <v>-334.94211816666666</v>
-      </c>
-      <c r="M15" s="2">
+        <v>1261.026196812807</v>
+      </c>
+      <c r="Q15" s="2">
         <f t="shared" si="3"/>
-        <v>78769.416628974373</v>
-      </c>
-      <c r="N15" s="2">
+        <v>610.02678479954136</v>
+      </c>
+      <c r="R15" s="2">
         <f t="shared" si="4"/>
-        <v>112186.22252197329</v>
-      </c>
-      <c r="O15" s="2">
+        <v>1.9403459193690049</v>
+      </c>
+      <c r="S15" s="2">
+        <f>(K15-H$2)*(K15-H$2)</f>
+        <v>1361.8973677606402</v>
+      </c>
+      <c r="T15" s="2">
         <f t="shared" si="5"/>
-        <v>94004.485541191825</v>
-      </c>
-      <c r="P15" s="2">
+        <v>1.3929630000000017</v>
+      </c>
+      <c r="U15">
+        <v>4.0966670000000001</v>
+      </c>
+      <c r="V15">
+        <v>3.8112159999999999</v>
+      </c>
+      <c r="W15">
         <f t="shared" si="6"/>
-        <v>801.89836319610049</v>
-      </c>
-      <c r="Q15" s="2">
-        <f t="shared" si="7"/>
-        <v>94018.466358686957</v>
-      </c>
-      <c r="R15" s="2">
-        <f t="shared" si="8"/>
-        <v>28.317810000000009</v>
-      </c>
-      <c r="S15">
-        <v>4.0966670000000001</v>
-      </c>
-      <c r="T15">
-        <v>3.8112159999999999</v>
-      </c>
-      <c r="U15">
-        <f t="shared" si="9"/>
         <v>-0.28545100000000012</v>
       </c>
-      <c r="V15"/>
-      <c r="W15">
+      <c r="Y15">
         <v>5.3976810000000004</v>
       </c>
-      <c r="X15">
+      <c r="Z15">
         <v>5.5303319999999996</v>
       </c>
-      <c r="Y15">
+      <c r="AA15">
         <v>5.5303319999999996</v>
       </c>
-      <c r="Z15">
+      <c r="AB15">
         <v>7.4527349999999997</v>
       </c>
-      <c r="AA15">
+      <c r="AC15">
         <v>5.3976810000000004</v>
       </c>
-      <c r="AC15">
+      <c r="AE15">
         <v>4.1435750000000002</v>
       </c>
-      <c r="AD15">
+      <c r="AF15">
         <v>5.272043</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="D16">
         <v>12</v>
       </c>
@@ -8597,61 +8620,62 @@
       <c r="G16">
         <v>31</v>
       </c>
-      <c r="H16">
-        <v>1263.4288329999999</v>
-      </c>
-      <c r="I16">
-        <v>1170.87085</v>
-      </c>
-      <c r="J16" s="2">
-        <f t="shared" ref="J16:J27" si="10">I16-H16</f>
-        <v>-92.557982999999922</v>
-      </c>
-      <c r="K16" s="2">
-        <f t="shared" ref="K16:K27" si="11">I16-I$2</f>
-        <v>353.87186470833319</v>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16">
+        <v>141.38772599999999</v>
+      </c>
+      <c r="K16">
+        <v>137.00288399999999</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" ref="L16:L27" si="12">H16-H$2</f>
-        <v>420.46443683333325</v>
+        <f t="shared" ref="L16:L27" si="7">K16-J16</f>
+        <v>-4.3848419999999919</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" ref="M16:M27" si="13">K16*K16</f>
-        <v>125225.29663215287</v>
+        <f>K16-I$2</f>
+        <v>70.993097291666658</v>
       </c>
       <c r="N16" s="2">
-        <f t="shared" ref="N16:N27" si="14">L16*L16</f>
-        <v>176790.34264157209</v>
+        <f>J16-H$2</f>
+        <v>55.652609333333316</v>
       </c>
       <c r="O16" s="2">
-        <f t="shared" ref="O16:O27" si="15">K16*L16</f>
-        <v>148790.5343057508</v>
+        <f t="shared" ref="O16:O27" si="8">M16*M16</f>
+        <v>5040.019863064048</v>
       </c>
       <c r="P16" s="2">
-        <f t="shared" ref="P16:P27" si="16">J16*J16</f>
-        <v>8566.9802170282746</v>
+        <f t="shared" ref="P16:P27" si="9">N16*N16</f>
+        <v>3097.2129256086187</v>
       </c>
       <c r="Q16" s="2">
-        <f t="shared" ref="Q16:Q27" si="17">(I16-H$2)*(I16-H$2)</f>
-        <v>107522.64246555197</v>
+        <f t="shared" ref="Q16:Q27" si="10">M16*N16</f>
+        <v>3950.9511089364482</v>
       </c>
       <c r="R16" s="2">
-        <f t="shared" ref="R16:R27" si="18">ABS(J16)</f>
-        <v>92.557982999999922</v>
-      </c>
-      <c r="S16">
+        <f t="shared" ref="R16:R27" si="11">L16*L16</f>
+        <v>19.226839364963929</v>
+      </c>
+      <c r="S16" s="2">
+        <f>(K16-H$2)*(K16-H$2)</f>
+        <v>2628.3839673447997</v>
+      </c>
+      <c r="T16" s="2">
+        <f t="shared" ref="T16:T27" si="12">ABS(L16)</f>
+        <v>4.3848419999999919</v>
+      </c>
+      <c r="U16">
         <v>4.4663490000000001</v>
       </c>
-      <c r="T16">
+      <c r="V16">
         <v>5.4185150000000002</v>
       </c>
-      <c r="U16">
-        <f t="shared" ref="U16:U27" si="19">T16-S16</f>
+      <c r="W16">
+        <f t="shared" ref="W16:W27" si="13">V16-U16</f>
         <v>0.95216600000000007</v>
       </c>
-      <c r="V16"/>
-    </row>
-    <row r="17" spans="4:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D17">
         <v>13</v>
       </c>
@@ -8664,61 +8688,62 @@
       <c r="G17">
         <v>29</v>
       </c>
-      <c r="H17">
-        <v>1465.9085689999999</v>
-      </c>
-      <c r="I17">
-        <v>1254.3043210000001</v>
-      </c>
-      <c r="J17" s="2">
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17">
+        <v>171.355637</v>
+      </c>
+      <c r="K17">
+        <v>131.610962</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="7"/>
+        <v>-39.744675000000001</v>
+      </c>
+      <c r="M17" s="2">
+        <f>K17-I$2</f>
+        <v>65.601175291666664</v>
+      </c>
+      <c r="N17" s="2">
+        <f>J17-H$2</f>
+        <v>85.620520333333332</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="8"/>
+        <v>4303.514199647977</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="9"/>
+        <v>7330.8735021507464</v>
+      </c>
+      <c r="Q17" s="2">
         <f t="shared" si="10"/>
-        <v>-211.60424799999987</v>
-      </c>
-      <c r="K17" s="2">
+        <v>5616.8067629507095</v>
+      </c>
+      <c r="R17" s="2">
         <f t="shared" si="11"/>
-        <v>437.30533570833325</v>
-      </c>
-      <c r="L17" s="2">
+        <v>1579.639190855625</v>
+      </c>
+      <c r="S17" s="2">
+        <f>(K17-H$2)*(K17-H$2)</f>
+        <v>2104.5931850479215</v>
+      </c>
+      <c r="T17" s="2">
         <f t="shared" si="12"/>
-        <v>622.94417283333325</v>
-      </c>
-      <c r="M17" s="2">
+        <v>39.744675000000001</v>
+      </c>
+      <c r="U17">
+        <v>4.6956059999999997</v>
+      </c>
+      <c r="V17">
+        <v>5.7108840000000001</v>
+      </c>
+      <c r="W17">
         <f t="shared" si="13"/>
-        <v>191235.95663897804</v>
-      </c>
-      <c r="N17" s="2">
-        <f t="shared" si="14"/>
-        <v>388059.44246700575</v>
-      </c>
-      <c r="O17" s="2">
-        <f t="shared" si="15"/>
-        <v>272416.81062843074</v>
-      </c>
-      <c r="P17" s="2">
-        <f t="shared" si="16"/>
-        <v>44776.357771645446</v>
-      </c>
-      <c r="Q17" s="2">
-        <f t="shared" si="17"/>
-        <v>169200.53376189235</v>
-      </c>
-      <c r="R17" s="2">
-        <f t="shared" si="18"/>
-        <v>211.60424799999987</v>
-      </c>
-      <c r="S17">
-        <v>4.6956059999999997</v>
-      </c>
-      <c r="T17">
-        <v>5.7108840000000001</v>
-      </c>
-      <c r="U17">
-        <f t="shared" si="19"/>
         <v>1.0152780000000003</v>
       </c>
-      <c r="V17"/>
-    </row>
-    <row r="18" spans="4:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D18">
         <v>14</v>
       </c>
@@ -8731,61 +8756,62 @@
       <c r="G18">
         <v>31</v>
       </c>
-      <c r="H18">
-        <v>912.38482699999997</v>
-      </c>
-      <c r="I18">
-        <v>690.69152799999995</v>
-      </c>
-      <c r="J18" s="2">
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18">
+        <v>115.339249</v>
+      </c>
+      <c r="K18">
+        <v>60.719954999999999</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="7"/>
+        <v>-54.619293999999996</v>
+      </c>
+      <c r="M18" s="2">
+        <f>K18-I$2</f>
+        <v>-5.2898317083333382</v>
+      </c>
+      <c r="N18" s="2">
+        <f>J18-H$2</f>
+        <v>29.604132333333325</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="8"/>
+        <v>27.982319502488803</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="9"/>
+        <v>876.4046512095116</v>
+      </c>
+      <c r="Q18" s="2">
         <f t="shared" si="10"/>
-        <v>-221.69329900000002</v>
-      </c>
-      <c r="K18" s="2">
+        <v>-156.60087791456283</v>
+      </c>
+      <c r="R18" s="2">
         <f t="shared" si="11"/>
-        <v>-126.30745729166688</v>
-      </c>
-      <c r="L18" s="2">
+        <v>2983.2672770584354</v>
+      </c>
+      <c r="S18" s="2">
+        <f>(K18-H$2)*(K18-H$2)</f>
+        <v>625.75831320946963</v>
+      </c>
+      <c r="T18" s="2">
         <f t="shared" si="12"/>
-        <v>69.420430833333285</v>
-      </c>
-      <c r="M18" s="2">
+        <v>54.619293999999996</v>
+      </c>
+      <c r="U18">
+        <v>5.3733880000000003</v>
+      </c>
+      <c r="V18">
+        <v>5.9636950000000004</v>
+      </c>
+      <c r="W18">
         <f t="shared" si="13"/>
-        <v>15953.573767486252</v>
-      </c>
-      <c r="N18" s="2">
-        <f t="shared" si="14"/>
-        <v>4819.1962170856104</v>
-      </c>
-      <c r="O18" s="2">
-        <f t="shared" si="15"/>
-        <v>-8768.3181026503589</v>
-      </c>
-      <c r="P18" s="2">
-        <f t="shared" si="16"/>
-        <v>49147.918821503408</v>
-      </c>
-      <c r="Q18" s="2">
-        <f t="shared" si="17"/>
-        <v>23187.026379703068</v>
-      </c>
-      <c r="R18" s="2">
-        <f t="shared" si="18"/>
-        <v>221.69329900000002</v>
-      </c>
-      <c r="S18">
-        <v>5.3733880000000003</v>
-      </c>
-      <c r="T18">
-        <v>5.9636950000000004</v>
-      </c>
-      <c r="U18">
-        <f t="shared" si="19"/>
         <v>0.59030700000000014</v>
       </c>
-      <c r="V18"/>
-    </row>
-    <row r="19" spans="4:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D19">
         <v>15</v>
       </c>
@@ -8798,61 +8824,62 @@
       <c r="G19">
         <v>30</v>
       </c>
-      <c r="H19">
-        <v>1197.2650149999999</v>
-      </c>
-      <c r="I19">
-        <v>1226.988159</v>
-      </c>
-      <c r="J19" s="2">
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19">
+        <v>103.370659</v>
+      </c>
+      <c r="K19">
+        <v>148.37773100000001</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="7"/>
+        <v>45.007072000000008</v>
+      </c>
+      <c r="M19" s="2">
+        <f>K19-I$2</f>
+        <v>82.367944291666674</v>
+      </c>
+      <c r="N19" s="2">
+        <f>J19-H$2</f>
+        <v>17.635542333333333</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="8"/>
+        <v>6784.478246835105</v>
+      </c>
+      <c r="P19" s="2">
+        <f t="shared" si="9"/>
+        <v>311.0123533907921</v>
+      </c>
+      <c r="Q19" s="2">
         <f t="shared" si="10"/>
-        <v>29.723144000000048</v>
-      </c>
-      <c r="K19" s="2">
+        <v>1452.6033684653294</v>
+      </c>
+      <c r="R19" s="2">
         <f t="shared" si="11"/>
-        <v>409.98917370833317</v>
-      </c>
-      <c r="L19" s="2">
+        <v>2025.6365300131847</v>
+      </c>
+      <c r="S19" s="2">
+        <f>(K19-H$2)*(K19-H$2)</f>
+        <v>3924.09713051474</v>
+      </c>
+      <c r="T19" s="2">
         <f t="shared" si="12"/>
-        <v>354.30061883333326</v>
-      </c>
-      <c r="M19" s="2">
+        <v>45.007072000000008</v>
+      </c>
+      <c r="U19">
+        <v>6.4953919999999998</v>
+      </c>
+      <c r="V19">
+        <v>7.5892429999999997</v>
+      </c>
+      <c r="W19">
         <f t="shared" si="13"/>
-        <v>168091.1225580418</v>
-      </c>
-      <c r="N19" s="2">
-        <f t="shared" si="14"/>
-        <v>125528.9285056829</v>
-      </c>
-      <c r="O19" s="2">
-        <f t="shared" si="15"/>
-        <v>145259.41795982941</v>
-      </c>
-      <c r="P19" s="2">
-        <f t="shared" si="16"/>
-        <v>883.46528924473887</v>
-      </c>
-      <c r="Q19" s="2">
-        <f t="shared" si="17"/>
-        <v>147474.25042067224</v>
-      </c>
-      <c r="R19" s="2">
-        <f t="shared" si="18"/>
-        <v>29.723144000000048</v>
-      </c>
-      <c r="S19">
-        <v>6.4953919999999998</v>
-      </c>
-      <c r="T19">
-        <v>7.5892429999999997</v>
-      </c>
-      <c r="U19">
-        <f t="shared" si="19"/>
         <v>1.0938509999999999</v>
       </c>
-      <c r="V19"/>
-    </row>
-    <row r="20" spans="4:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D20">
         <v>16</v>
       </c>
@@ -8865,61 +8892,62 @@
       <c r="G20">
         <v>31</v>
       </c>
-      <c r="H20">
-        <v>999.23718299999996</v>
-      </c>
-      <c r="I20">
-        <v>1157.6922609999999</v>
-      </c>
-      <c r="J20" s="2">
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20">
+        <v>86.076751999999999</v>
+      </c>
+      <c r="K20">
+        <v>104.30669399999999</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="7"/>
+        <v>18.229941999999994</v>
+      </c>
+      <c r="M20" s="2">
+        <f>K20-I$2</f>
+        <v>38.296907291666656</v>
+      </c>
+      <c r="N20" s="2">
+        <f>J20-H$2</f>
+        <v>0.34163533333332907</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="8"/>
+        <v>1466.6531081065107</v>
+      </c>
+      <c r="P20" s="2">
+        <f t="shared" si="9"/>
+        <v>0.11671470098177486</v>
+      </c>
+      <c r="Q20" s="2">
         <f t="shared" si="10"/>
-        <v>158.45507799999996</v>
-      </c>
-      <c r="K20" s="2">
+        <v>13.083576688224138</v>
+      </c>
+      <c r="R20" s="2">
         <f t="shared" si="11"/>
-        <v>340.69327570833309</v>
-      </c>
-      <c r="L20" s="2">
+        <v>332.33078532336378</v>
+      </c>
+      <c r="S20" s="2">
+        <f>(K20-H$2)*(K20-H$2)</f>
+        <v>344.90348464798006</v>
+      </c>
+      <c r="T20" s="2">
         <f t="shared" si="12"/>
-        <v>156.27278683333327</v>
-      </c>
-      <c r="M20" s="2">
+        <v>18.229941999999994</v>
+      </c>
+      <c r="U20">
+        <v>9.6104040000000008</v>
+      </c>
+      <c r="V20">
+        <v>11.136310999999999</v>
+      </c>
+      <c r="W20">
         <f t="shared" si="13"/>
-        <v>116071.90811287427</v>
-      </c>
-      <c r="N20" s="2">
-        <f t="shared" si="14"/>
-        <v>24421.18390465642</v>
-      </c>
-      <c r="O20" s="2">
-        <f t="shared" si="15"/>
-        <v>53241.087650318375</v>
-      </c>
-      <c r="P20" s="2">
-        <f t="shared" si="16"/>
-        <v>25108.01174398607</v>
-      </c>
-      <c r="Q20" s="2">
-        <f t="shared" si="17"/>
-        <v>99053.628902548866</v>
-      </c>
-      <c r="R20" s="2">
-        <f t="shared" si="18"/>
-        <v>158.45507799999996</v>
-      </c>
-      <c r="S20">
-        <v>9.6104040000000008</v>
-      </c>
-      <c r="T20">
-        <v>11.136310999999999</v>
-      </c>
-      <c r="U20">
-        <f t="shared" si="19"/>
         <v>1.5259069999999983</v>
       </c>
-      <c r="V20"/>
-    </row>
-    <row r="21" spans="4:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D21">
         <v>17</v>
       </c>
@@ -8932,61 +8960,62 @@
       <c r="G21">
         <v>30</v>
       </c>
-      <c r="H21">
-        <v>679.75945999999999</v>
-      </c>
-      <c r="I21">
-        <v>827.918274</v>
-      </c>
-      <c r="J21" s="2">
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21">
+        <v>85.735054000000005</v>
+      </c>
+      <c r="K21">
+        <v>57.712505</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="7"/>
+        <v>-28.022549000000005</v>
+      </c>
+      <c r="M21" s="2">
+        <f>K21-I$2</f>
+        <v>-8.2972817083333368</v>
+      </c>
+      <c r="N21" s="2">
+        <f>J21-H$2</f>
+        <v>-6.2666666664767945E-5</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="8"/>
+        <v>68.844883747442978</v>
+      </c>
+      <c r="P21" s="2">
+        <f t="shared" si="9"/>
+        <v>3.9271111108731378E-9</v>
+      </c>
+      <c r="Q21" s="2">
         <f t="shared" si="10"/>
-        <v>148.15881400000001</v>
-      </c>
-      <c r="K21" s="2">
+        <v>5.1996298703980157E-4</v>
+      </c>
+      <c r="R21" s="2">
         <f t="shared" si="11"/>
-        <v>10.91928870833317</v>
-      </c>
-      <c r="L21" s="2">
+        <v>785.26325245740134</v>
+      </c>
+      <c r="S21" s="2">
+        <f>(K21-H$2)*(K21-H$2)</f>
+        <v>785.26676462080297</v>
+      </c>
+      <c r="T21" s="2">
         <f t="shared" si="12"/>
-        <v>-163.2049361666667</v>
-      </c>
-      <c r="M21" s="2">
+        <v>28.022549000000005</v>
+      </c>
+      <c r="U21">
+        <v>10.771552</v>
+      </c>
+      <c r="V21">
+        <v>12.600471000000001</v>
+      </c>
+      <c r="W21">
         <f t="shared" si="13"/>
-        <v>119.23086589593227</v>
-      </c>
-      <c r="N21" s="2">
-        <f t="shared" si="14"/>
-        <v>26635.851189165751</v>
-      </c>
-      <c r="O21" s="2">
-        <f t="shared" si="15"/>
-        <v>-1782.0818166289193</v>
-      </c>
-      <c r="P21" s="2">
-        <f t="shared" si="16"/>
-        <v>21951.034165886598</v>
-      </c>
-      <c r="Q21" s="2">
-        <f t="shared" si="17"/>
-        <v>226.38579225425877</v>
-      </c>
-      <c r="R21" s="2">
-        <f t="shared" si="18"/>
-        <v>148.15881400000001</v>
-      </c>
-      <c r="S21">
-        <v>10.771552</v>
-      </c>
-      <c r="T21">
-        <v>12.600471000000001</v>
-      </c>
-      <c r="U21">
-        <f t="shared" si="19"/>
         <v>1.8289190000000008</v>
       </c>
-      <c r="V21"/>
-    </row>
-    <row r="22" spans="4:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D22">
         <v>18</v>
       </c>
@@ -8999,61 +9028,62 @@
       <c r="G22">
         <v>31</v>
       </c>
-      <c r="H22">
-        <v>423.25503500000002</v>
-      </c>
-      <c r="I22">
-        <v>526.04125999999997</v>
-      </c>
-      <c r="J22" s="2">
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22">
+        <v>38.052138999999997</v>
+      </c>
+      <c r="K22">
+        <v>13.518675</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="7"/>
+        <v>-24.533463999999995</v>
+      </c>
+      <c r="M22" s="2">
+        <f>K22-I$2</f>
+        <v>-52.491111708333335</v>
+      </c>
+      <c r="N22" s="2">
+        <f>J22-H$2</f>
+        <v>-47.682977666666673</v>
+      </c>
+      <c r="O22" s="2">
+        <f t="shared" si="8"/>
+        <v>2755.3168083767291</v>
+      </c>
+      <c r="P22" s="2">
+        <f t="shared" si="9"/>
+        <v>2273.6663591598326</v>
+      </c>
+      <c r="Q22" s="2">
         <f t="shared" si="10"/>
-        <v>102.78622499999994</v>
-      </c>
-      <c r="K22" s="2">
+        <v>2502.9325072869638</v>
+      </c>
+      <c r="R22" s="2">
         <f t="shared" si="11"/>
-        <v>-290.95772529166686</v>
-      </c>
-      <c r="L22" s="2">
+        <v>601.8908558392958</v>
+      </c>
+      <c r="S22" s="2">
+        <f>(K22-H$2)*(K22-H$2)</f>
+        <v>5215.2144469950699</v>
+      </c>
+      <c r="T22" s="2">
         <f t="shared" si="12"/>
-        <v>-419.70936116666667</v>
-      </c>
-      <c r="M22" s="2">
+        <v>24.533463999999995</v>
+      </c>
+      <c r="U22">
+        <v>13.215975</v>
+      </c>
+      <c r="V22">
+        <v>15.246349</v>
+      </c>
+      <c r="W22">
         <f t="shared" si="13"/>
-        <v>84656.397906901082</v>
-      </c>
-      <c r="N22" s="2">
-        <f t="shared" si="14"/>
-        <v>176155.94785093144</v>
-      </c>
-      <c r="O22" s="2">
-        <f t="shared" si="15"/>
-        <v>122117.68100867199</v>
-      </c>
-      <c r="P22" s="2">
-        <f t="shared" si="16"/>
-        <v>10565.008049750613</v>
-      </c>
-      <c r="Q22" s="2">
-        <f t="shared" si="17"/>
-        <v>100440.27423771558</v>
-      </c>
-      <c r="R22" s="2">
-        <f t="shared" si="18"/>
-        <v>102.78622499999994</v>
-      </c>
-      <c r="S22">
-        <v>13.215975</v>
-      </c>
-      <c r="T22">
-        <v>15.246349</v>
-      </c>
-      <c r="U22">
-        <f t="shared" si="19"/>
         <v>2.0303740000000001</v>
       </c>
-      <c r="V22"/>
-    </row>
-    <row r="23" spans="4:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D23">
         <v>19</v>
       </c>
@@ -9066,61 +9096,62 @@
       <c r="G23">
         <v>31</v>
       </c>
-      <c r="H23">
-        <v>356.11215199999998</v>
-      </c>
-      <c r="I23">
-        <v>416.39163200000002</v>
-      </c>
-      <c r="J23" s="2">
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23">
+        <v>29.898626</v>
+      </c>
+      <c r="K23">
+        <v>4.8387399999999996</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="7"/>
+        <v>-25.059885999999999</v>
+      </c>
+      <c r="M23" s="2">
+        <f>K23-I$2</f>
+        <v>-61.171046708333336</v>
+      </c>
+      <c r="N23" s="2">
+        <f>J23-H$2</f>
+        <v>-55.83649066666667</v>
+      </c>
+      <c r="O23" s="2">
+        <f t="shared" si="8"/>
+        <v>3741.8969553930988</v>
+      </c>
+      <c r="P23" s="2">
+        <f t="shared" si="9"/>
+        <v>3117.7136899687544</v>
+      </c>
+      <c r="Q23" s="2">
         <f t="shared" si="10"/>
-        <v>60.279480000000035</v>
-      </c>
-      <c r="K23" s="2">
+        <v>3415.5765786000852</v>
+      </c>
+      <c r="R23" s="2">
         <f t="shared" si="11"/>
-        <v>-400.60735329166681</v>
-      </c>
-      <c r="L23" s="2">
+        <v>627.9978863329959</v>
+      </c>
+      <c r="S23" s="2">
+        <f>(K23-H$2)*(K23-H$2)</f>
+        <v>6544.223757795211</v>
+      </c>
+      <c r="T23" s="2">
         <f t="shared" si="12"/>
-        <v>-486.85224416666671</v>
-      </c>
-      <c r="M23" s="2">
+        <v>25.059885999999999</v>
+      </c>
+      <c r="U23">
+        <v>15.243527</v>
+      </c>
+      <c r="V23">
+        <v>17.401871</v>
+      </c>
+      <c r="W23">
         <f t="shared" si="13"/>
-        <v>160486.25151135435</v>
-      </c>
-      <c r="N23" s="2">
-        <f t="shared" si="14"/>
-        <v>237025.10765011967</v>
-      </c>
-      <c r="O23" s="2">
-        <f t="shared" si="15"/>
-        <v>195036.58897971667</v>
-      </c>
-      <c r="P23" s="2">
-        <f t="shared" si="16"/>
-        <v>3633.6157090704041</v>
-      </c>
-      <c r="Q23" s="2">
-        <f t="shared" si="17"/>
-        <v>181964.32312879062</v>
-      </c>
-      <c r="R23" s="2">
-        <f t="shared" si="18"/>
-        <v>60.279480000000035</v>
-      </c>
-      <c r="S23">
-        <v>15.243527</v>
-      </c>
-      <c r="T23">
-        <v>17.401871</v>
-      </c>
-      <c r="U23">
-        <f t="shared" si="19"/>
         <v>2.1583439999999996</v>
       </c>
-      <c r="V23"/>
-    </row>
-    <row r="24" spans="4:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D24">
         <v>20</v>
       </c>
@@ -9133,61 +9164,62 @@
       <c r="G24">
         <v>30</v>
       </c>
-      <c r="H24">
-        <v>336.58340500000003</v>
-      </c>
-      <c r="I24">
-        <v>381.95684799999998</v>
-      </c>
-      <c r="J24" s="2">
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24">
+        <v>29.81213</v>
+      </c>
+      <c r="K24">
+        <v>4.014062</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="7"/>
+        <v>-25.798068000000001</v>
+      </c>
+      <c r="M24" s="2">
+        <f>K24-I$2</f>
+        <v>-61.995724708333334</v>
+      </c>
+      <c r="N24" s="2">
+        <f>J24-H$2</f>
+        <v>-55.922986666666674</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="8"/>
+        <v>3843.4698821114521</v>
+      </c>
+      <c r="P24" s="2">
+        <f t="shared" si="9"/>
+        <v>3127.3804377201786</v>
+      </c>
+      <c r="Q24" s="2">
         <f t="shared" si="10"/>
-        <v>45.373442999999952</v>
-      </c>
-      <c r="K24" s="2">
+        <v>3466.9860862544629</v>
+      </c>
+      <c r="R24" s="2">
         <f t="shared" si="11"/>
-        <v>-435.04213729166685</v>
-      </c>
-      <c r="L24" s="2">
+        <v>665.54031253262406</v>
+      </c>
+      <c r="S24" s="2">
+        <f>(K24-H$2)*(K24-H$2)</f>
+        <v>6678.3307758323226</v>
+      </c>
+      <c r="T24" s="2">
         <f t="shared" si="12"/>
-        <v>-506.38099116666666</v>
-      </c>
-      <c r="M24" s="2">
+        <v>25.798068000000001</v>
+      </c>
+      <c r="U24">
+        <v>14.913529</v>
+      </c>
+      <c r="V24">
+        <v>17.110749999999999</v>
+      </c>
+      <c r="W24">
         <f t="shared" si="13"/>
-        <v>189261.66121930152</v>
-      </c>
-      <c r="N24" s="2">
-        <f t="shared" si="14"/>
-        <v>256421.70821493573</v>
-      </c>
-      <c r="O24" s="2">
-        <f t="shared" si="15"/>
-        <v>220297.06868101933</v>
-      </c>
-      <c r="P24" s="2">
-        <f t="shared" si="16"/>
-        <v>2058.7493296742446</v>
-      </c>
-      <c r="Q24" s="2">
-        <f t="shared" si="17"/>
-        <v>212527.95946664154</v>
-      </c>
-      <c r="R24" s="2">
-        <f t="shared" si="18"/>
-        <v>45.373442999999952</v>
-      </c>
-      <c r="S24">
-        <v>14.913529</v>
-      </c>
-      <c r="T24">
-        <v>17.110749999999999</v>
-      </c>
-      <c r="U24">
-        <f t="shared" si="19"/>
         <v>2.197220999999999</v>
       </c>
-      <c r="V24"/>
-    </row>
-    <row r="25" spans="4:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D25">
         <v>21</v>
       </c>
@@ -9200,61 +9232,62 @@
       <c r="G25">
         <v>31</v>
       </c>
-      <c r="H25">
-        <v>439.83184799999998</v>
-      </c>
-      <c r="I25">
-        <v>418.79754600000001</v>
-      </c>
-      <c r="J25" s="2">
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25">
+        <v>40.966869000000003</v>
+      </c>
+      <c r="K25">
+        <v>7.5922260000000001</v>
+      </c>
+      <c r="L25" s="2">
+        <f t="shared" si="7"/>
+        <v>-33.374643000000006</v>
+      </c>
+      <c r="M25" s="2">
+        <f>K25-I$2</f>
+        <v>-58.41756070833334</v>
+      </c>
+      <c r="N25" s="2">
+        <f>J25-H$2</f>
+        <v>-44.768247666666667</v>
+      </c>
+      <c r="O25" s="2">
+        <f t="shared" si="8"/>
+        <v>3412.6113991118114</v>
+      </c>
+      <c r="P25" s="2">
+        <f t="shared" si="9"/>
+        <v>2004.1959991440056</v>
+      </c>
+      <c r="Q25" s="2">
         <f t="shared" si="10"/>
-        <v>-21.034301999999968</v>
-      </c>
-      <c r="K25" s="2">
+        <v>2615.2518258732025</v>
+      </c>
+      <c r="R25" s="2">
         <f t="shared" si="11"/>
-        <v>-398.20143929166682</v>
-      </c>
-      <c r="L25" s="2">
+        <v>1113.8667953774493</v>
+      </c>
+      <c r="S25" s="2">
+        <f>(K25-H$2)*(K25-H$2)</f>
+        <v>6106.3113617426216</v>
+      </c>
+      <c r="T25" s="2">
         <f t="shared" si="12"/>
-        <v>-403.13254816666671</v>
-      </c>
-      <c r="M25" s="2">
+        <v>33.374643000000006</v>
+      </c>
+      <c r="U25">
+        <v>13.524543</v>
+      </c>
+      <c r="V25">
+        <v>15.616877000000001</v>
+      </c>
+      <c r="W25">
         <f t="shared" si="13"/>
-        <v>158564.38625395502</v>
-      </c>
-      <c r="N25" s="2">
-        <f t="shared" si="14"/>
-        <v>162515.85139134986</v>
-      </c>
-      <c r="O25" s="2">
-        <f t="shared" si="15"/>
-        <v>160527.96090528389</v>
-      </c>
-      <c r="P25" s="2">
-        <f t="shared" si="16"/>
-        <v>442.44186062720269</v>
-      </c>
-      <c r="Q25" s="2">
-        <f t="shared" si="17"/>
-        <v>179917.51678031145</v>
-      </c>
-      <c r="R25" s="2">
-        <f t="shared" si="18"/>
-        <v>21.034301999999968</v>
-      </c>
-      <c r="S25">
-        <v>13.524543</v>
-      </c>
-      <c r="T25">
-        <v>15.616877000000001</v>
-      </c>
-      <c r="U25">
-        <f t="shared" si="19"/>
         <v>2.092334000000001</v>
       </c>
-      <c r="V25"/>
-    </row>
-    <row r="26" spans="4:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D26">
         <v>22</v>
       </c>
@@ -9267,61 +9300,62 @@
       <c r="G26">
         <v>30</v>
       </c>
-      <c r="H26">
-        <v>772.81073000000004</v>
-      </c>
-      <c r="I26">
-        <v>742.23394800000005</v>
-      </c>
-      <c r="J26" s="2">
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26">
+        <v>86.169539999999998</v>
+      </c>
+      <c r="K26">
+        <v>61.275429000000003</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="7"/>
+        <v>-24.894110999999995</v>
+      </c>
+      <c r="M26" s="2">
+        <f>K26-I$2</f>
+        <v>-4.7343577083333344</v>
+      </c>
+      <c r="N26" s="2">
+        <f>J26-H$2</f>
+        <v>0.43442333333332783</v>
+      </c>
+      <c r="O26" s="2">
+        <f t="shared" si="8"/>
+        <v>22.414142910455261</v>
+      </c>
+      <c r="P26" s="2">
+        <f t="shared" si="9"/>
+        <v>0.18872363254443966</v>
+      </c>
+      <c r="Q26" s="2">
         <f t="shared" si="10"/>
-        <v>-30.57678199999998</v>
-      </c>
-      <c r="K26" s="2">
+        <v>-2.056715456846502</v>
+      </c>
+      <c r="R26" s="2">
         <f t="shared" si="11"/>
-        <v>-74.765037291666772</v>
-      </c>
-      <c r="L26" s="2">
+        <v>619.71676248032077</v>
+      </c>
+      <c r="S26" s="2">
+        <f>(K26-H$2)*(K26-H$2)</f>
+        <v>598.27632075088547</v>
+      </c>
+      <c r="T26" s="2">
         <f t="shared" si="12"/>
-        <v>-70.153666166666653</v>
-      </c>
-      <c r="M26" s="2">
+        <v>24.894110999999995</v>
+      </c>
+      <c r="U26">
+        <v>7.9147090000000002</v>
+      </c>
+      <c r="V26">
+        <v>9.3853279999999994</v>
+      </c>
+      <c r="W26">
         <f t="shared" si="13"/>
-        <v>5589.8108012243229</v>
-      </c>
-      <c r="N26" s="2">
-        <f t="shared" si="14"/>
-        <v>4921.536876624109</v>
-      </c>
-      <c r="O26" s="2">
-        <f t="shared" si="15"/>
-        <v>5245.0414670979735</v>
-      </c>
-      <c r="P26" s="2">
-        <f t="shared" si="16"/>
-        <v>934.93959747552276</v>
-      </c>
-      <c r="Q26" s="2">
-        <f t="shared" si="17"/>
-        <v>10146.623187857513</v>
-      </c>
-      <c r="R26" s="2">
-        <f t="shared" si="18"/>
-        <v>30.57678199999998</v>
-      </c>
-      <c r="S26">
-        <v>7.9147090000000002</v>
-      </c>
-      <c r="T26">
-        <v>9.3853279999999994</v>
-      </c>
-      <c r="U26">
-        <f t="shared" si="19"/>
         <v>1.4706189999999992</v>
       </c>
-      <c r="V26"/>
-    </row>
-    <row r="27" spans="4:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D27">
         <v>23</v>
       </c>
@@ -9334,61 +9368,62 @@
       <c r="G27">
         <v>31</v>
       </c>
-      <c r="H27">
-        <v>1337.5745850000001</v>
-      </c>
-      <c r="I27">
-        <v>1301.7392580000001</v>
-      </c>
-      <c r="J27" s="2">
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27">
+        <v>174.08557099999999</v>
+      </c>
+      <c r="K27">
+        <v>148.006989</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="7"/>
+        <v>-26.078581999999983</v>
+      </c>
+      <c r="M27" s="2">
+        <f>K27-I$2</f>
+        <v>81.997202291666667</v>
+      </c>
+      <c r="N27" s="2">
+        <f>J27-H$2</f>
+        <v>88.350454333333317</v>
+      </c>
+      <c r="O27" s="2">
+        <f t="shared" si="8"/>
+        <v>6723.5411836605053</v>
+      </c>
+      <c r="P27" s="2">
+        <f t="shared" si="9"/>
+        <v>7805.802780906416</v>
+      </c>
+      <c r="Q27" s="2">
         <f t="shared" si="10"/>
-        <v>-35.835327000000007</v>
-      </c>
-      <c r="K27" s="2">
+        <v>7244.4900765309903</v>
+      </c>
+      <c r="R27" s="2">
         <f t="shared" si="11"/>
-        <v>484.74027270833324</v>
-      </c>
-      <c r="L27" s="2">
+        <v>680.09243913072316</v>
+      </c>
+      <c r="S27" s="2">
+        <f>(K27-H$2)*(K27-H$2)</f>
+        <v>3877.7860838989654</v>
+      </c>
+      <c r="T27" s="2">
         <f t="shared" si="12"/>
-        <v>494.61018883333338</v>
-      </c>
-      <c r="M27" s="2">
+        <v>26.078581999999983</v>
+      </c>
+      <c r="U27">
+        <v>4.2786520000000001</v>
+      </c>
+      <c r="V27">
+        <v>4.3472080000000002</v>
+      </c>
+      <c r="W27">
         <f t="shared" si="13"/>
-        <v>234973.13198534929</v>
-      </c>
-      <c r="N27" s="2">
-        <f t="shared" si="14"/>
-        <v>244639.2388977457</v>
-      </c>
-      <c r="O27" s="2">
-        <f t="shared" si="15"/>
-        <v>239757.47781939022</v>
-      </c>
-      <c r="P27" s="2">
-        <f t="shared" si="16"/>
-        <v>1284.1706611969294</v>
-      </c>
-      <c r="Q27" s="2">
-        <f t="shared" si="17"/>
-        <v>210474.37385019413</v>
-      </c>
-      <c r="R27" s="2">
-        <f t="shared" si="18"/>
-        <v>35.835327000000007</v>
-      </c>
-      <c r="S27">
-        <v>4.2786520000000001</v>
-      </c>
-      <c r="T27">
-        <v>4.3472080000000002</v>
-      </c>
-      <c r="U27">
-        <f t="shared" si="19"/>
         <v>6.8556000000000061E-2</v>
       </c>
-      <c r="V27"/>
-    </row>
-    <row r="28" spans="4:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="4:23" x14ac:dyDescent="0.3">
       <c r="H28"/>
       <c r="I28"/>
       <c r="S28"/>
@@ -9396,7 +9431,7 @@
       <c r="U28"/>
       <c r="V28"/>
     </row>
-    <row r="29" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:23" x14ac:dyDescent="0.3">
       <c r="H29"/>
       <c r="I29"/>
       <c r="S29"/>
@@ -9404,7 +9439,7 @@
       <c r="U29"/>
       <c r="V29"/>
     </row>
-    <row r="30" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:23" x14ac:dyDescent="0.3">
       <c r="H30"/>
       <c r="I30"/>
       <c r="S30"/>
@@ -9412,7 +9447,7 @@
       <c r="U30"/>
       <c r="V30"/>
     </row>
-    <row r="31" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:23" x14ac:dyDescent="0.3">
       <c r="H31"/>
       <c r="I31"/>
       <c r="S31"/>
@@ -9420,7 +9455,7 @@
       <c r="U31"/>
       <c r="V31"/>
     </row>
-    <row r="32" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:23" x14ac:dyDescent="0.3">
       <c r="H32"/>
       <c r="I32"/>
       <c r="S32"/>

</xml_diff>